<commit_message>
pickup-deli real map added.
</commit_message>
<xml_diff>
--- a/real_map/DISTANCES.xlsx
+++ b/real_map/DISTANCES.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -332,10 +332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U21"/>
+  <dimension ref="B2:BI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:U21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AX15" sqref="AX15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1270,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>2923</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2331</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>2209</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>3130</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:61" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>3937</v>
       </c>
@@ -1577,10 +1577,4891 @@
         <v>983</v>
       </c>
       <c r="U21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1">
+        <v>1951</v>
+      </c>
+      <c r="X22" s="1">
+        <v>2513</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>2551</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>3451</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>3098</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>3250</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>5007</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>5658</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>5619</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>9296</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>5774</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>7313</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>7787</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>7928</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>9134</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>8375</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>9778</v>
+      </c>
+      <c r="AN22" s="1">
+        <v>7887</v>
+      </c>
+      <c r="AO22" s="1">
+        <v>9413</v>
+      </c>
+      <c r="AP22" s="1">
+        <v>7631</v>
+      </c>
+      <c r="AQ22" s="1">
+        <v>6290</v>
+      </c>
+      <c r="AR22" s="1">
+        <v>6320</v>
+      </c>
+      <c r="AS22" s="1">
+        <v>6424</v>
+      </c>
+      <c r="AT22" s="1">
+        <v>7537</v>
+      </c>
+      <c r="AU22" s="1">
+        <v>7258</v>
+      </c>
+      <c r="AV22" s="1">
+        <v>7546</v>
+      </c>
+      <c r="AW22" s="1">
+        <v>7975</v>
+      </c>
+      <c r="AX22" s="1">
+        <v>6356</v>
+      </c>
+      <c r="AY22" s="1">
+        <v>8057</v>
+      </c>
+      <c r="AZ22" s="1">
+        <v>8960</v>
+      </c>
+      <c r="BA22" s="1">
+        <v>8991</v>
+      </c>
+      <c r="BB22" s="1">
+        <v>6747</v>
+      </c>
+      <c r="BC22" s="1">
+        <v>9777</v>
+      </c>
+      <c r="BD22" s="1">
+        <v>9331</v>
+      </c>
+      <c r="BE22" s="1">
+        <v>12022</v>
+      </c>
+      <c r="BF22" s="1">
+        <v>10664</v>
+      </c>
+      <c r="BG22" s="1">
+        <v>13824</v>
+      </c>
+      <c r="BH22" s="1">
+        <v>13577</v>
+      </c>
+      <c r="BI22" s="1">
+        <v>14661</v>
+      </c>
+    </row>
+    <row r="23" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V23" s="1">
+        <v>2555</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>561</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>599</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>1499</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>1145</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>1297</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>3054</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>3706</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>3667</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>7344</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>3822</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>5361</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>5834</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>5976</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>7181</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>6423</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>7826</v>
+      </c>
+      <c r="AN23" s="1">
+        <v>5934</v>
+      </c>
+      <c r="AO23" s="1">
+        <v>7460</v>
+      </c>
+      <c r="AP23" s="1">
+        <v>5679</v>
+      </c>
+      <c r="AQ23" s="1">
+        <v>4337</v>
+      </c>
+      <c r="AR23" s="1">
+        <v>4367</v>
+      </c>
+      <c r="AS23" s="1">
+        <v>4472</v>
+      </c>
+      <c r="AT23" s="1">
+        <v>5585</v>
+      </c>
+      <c r="AU23" s="1">
+        <v>5306</v>
+      </c>
+      <c r="AV23" s="1">
+        <v>5594</v>
+      </c>
+      <c r="AW23" s="1">
+        <v>6023</v>
+      </c>
+      <c r="AX23" s="1">
+        <v>4404</v>
+      </c>
+      <c r="AY23" s="1">
+        <v>7547</v>
+      </c>
+      <c r="AZ23" s="1">
+        <v>9787</v>
+      </c>
+      <c r="BA23" s="1">
+        <v>9818</v>
+      </c>
+      <c r="BB23" s="1">
+        <v>12037</v>
+      </c>
+      <c r="BC23" s="1">
+        <v>10604</v>
+      </c>
+      <c r="BD23" s="1">
+        <v>10158</v>
+      </c>
+      <c r="BE23" s="1">
+        <v>12756</v>
+      </c>
+      <c r="BF23" s="1">
+        <v>11492</v>
+      </c>
+      <c r="BG23" s="1">
+        <v>14961</v>
+      </c>
+      <c r="BH23" s="1">
+        <v>14714</v>
+      </c>
+      <c r="BI23" s="1">
+        <v>15798</v>
+      </c>
+    </row>
+    <row r="24" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V24" s="1">
+        <v>2194</v>
+      </c>
+      <c r="W24" s="1">
+        <v>2092</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>237</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>1137</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>784</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>936</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>2693</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>3344</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>3305</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>6982</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>3460</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>4999</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>5473</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>5615</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>6820</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>6061</v>
+      </c>
+      <c r="AM24" s="1">
+        <v>7464</v>
+      </c>
+      <c r="AN24" s="1">
+        <v>5573</v>
+      </c>
+      <c r="AO24" s="1">
+        <v>7099</v>
+      </c>
+      <c r="AP24" s="1">
+        <v>5317</v>
+      </c>
+      <c r="AQ24" s="1">
+        <v>3976</v>
+      </c>
+      <c r="AR24" s="1">
+        <v>4006</v>
+      </c>
+      <c r="AS24" s="1">
+        <v>4110</v>
+      </c>
+      <c r="AT24" s="1">
+        <v>5223</v>
+      </c>
+      <c r="AU24" s="1">
+        <v>4944</v>
+      </c>
+      <c r="AV24" s="1">
+        <v>5233</v>
+      </c>
+      <c r="AW24" s="1">
+        <v>5661</v>
+      </c>
+      <c r="AX24" s="1">
+        <v>4042</v>
+      </c>
+      <c r="AY24" s="1">
+        <v>7186</v>
+      </c>
+      <c r="AZ24" s="1">
+        <v>9426</v>
+      </c>
+      <c r="BA24" s="1">
+        <v>9457</v>
+      </c>
+      <c r="BB24" s="1">
+        <v>11675</v>
+      </c>
+      <c r="BC24" s="1">
+        <v>10243</v>
+      </c>
+      <c r="BD24" s="1">
+        <v>9796</v>
+      </c>
+      <c r="BE24" s="1">
+        <v>12394</v>
+      </c>
+      <c r="BF24" s="1">
+        <v>11130</v>
+      </c>
+      <c r="BG24" s="1">
+        <v>14599</v>
+      </c>
+      <c r="BH24" s="1">
+        <v>14353</v>
+      </c>
+      <c r="BI24" s="1">
+        <v>15437</v>
+      </c>
+    </row>
+    <row r="25" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V25" s="1">
+        <v>1956</v>
+      </c>
+      <c r="W25" s="1">
+        <v>1855</v>
+      </c>
+      <c r="X25" s="1">
+        <v>1681</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>900</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>546</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>699</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>2456</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>3107</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>3068</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>6745</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>3223</v>
+      </c>
+      <c r="AH25" s="1">
+        <v>4762</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>5236</v>
+      </c>
+      <c r="AJ25" s="1">
+        <v>5377</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>6582</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>5824</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>7227</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>5335</v>
+      </c>
+      <c r="AO25" s="1">
+        <v>6862</v>
+      </c>
+      <c r="AP25" s="1">
+        <v>5080</v>
+      </c>
+      <c r="AQ25" s="1">
+        <v>3739</v>
+      </c>
+      <c r="AR25" s="1">
+        <v>3768</v>
+      </c>
+      <c r="AS25" s="1">
+        <v>3873</v>
+      </c>
+      <c r="AT25" s="1">
+        <v>4986</v>
+      </c>
+      <c r="AU25" s="1">
+        <v>4707</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>4995</v>
+      </c>
+      <c r="AW25" s="1">
+        <v>5424</v>
+      </c>
+      <c r="AX25" s="1">
+        <v>3805</v>
+      </c>
+      <c r="AY25" s="1">
+        <v>6948</v>
+      </c>
+      <c r="AZ25" s="1">
+        <v>9189</v>
+      </c>
+      <c r="BA25" s="1">
+        <v>9219</v>
+      </c>
+      <c r="BB25" s="1">
+        <v>11438</v>
+      </c>
+      <c r="BC25" s="1">
+        <v>10006</v>
+      </c>
+      <c r="BD25" s="1">
+        <v>9559</v>
+      </c>
+      <c r="BE25" s="1">
+        <v>12157</v>
+      </c>
+      <c r="BF25" s="1">
+        <v>10893</v>
+      </c>
+      <c r="BG25" s="1">
+        <v>14362</v>
+      </c>
+      <c r="BH25" s="1">
+        <v>14116</v>
+      </c>
+      <c r="BI25" s="1">
+        <v>15200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V26" s="1">
+        <v>1056</v>
+      </c>
+      <c r="W26" s="1">
+        <v>955</v>
+      </c>
+      <c r="X26" s="1">
+        <v>1515</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>1554</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>2100</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>2252</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>4009</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>4660</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>4621</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>8298</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>4777</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>6315</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>6789</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>6931</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>8136</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>7377</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>8780</v>
+      </c>
+      <c r="AN26" s="1">
+        <v>6889</v>
+      </c>
+      <c r="AO26" s="1">
+        <v>8415</v>
+      </c>
+      <c r="AP26" s="1">
+        <v>6634</v>
+      </c>
+      <c r="AQ26" s="1">
+        <v>5292</v>
+      </c>
+      <c r="AR26" s="1">
+        <v>5322</v>
+      </c>
+      <c r="AS26" s="1">
+        <v>5427</v>
+      </c>
+      <c r="AT26" s="1">
+        <v>6539</v>
+      </c>
+      <c r="AU26" s="1">
+        <v>6261</v>
+      </c>
+      <c r="AV26" s="1">
+        <v>6549</v>
+      </c>
+      <c r="AW26" s="1">
+        <v>6978</v>
+      </c>
+      <c r="AX26" s="1">
+        <v>5358</v>
+      </c>
+      <c r="AY26" s="1">
+        <v>9115</v>
+      </c>
+      <c r="AZ26" s="1">
+        <v>10018</v>
+      </c>
+      <c r="BA26" s="1">
+        <v>10049</v>
+      </c>
+      <c r="BB26" s="1">
+        <v>7805</v>
+      </c>
+      <c r="BC26" s="1">
+        <v>10835</v>
+      </c>
+      <c r="BD26" s="1">
+        <v>10389</v>
+      </c>
+      <c r="BE26" s="1">
+        <v>13080</v>
+      </c>
+      <c r="BF26" s="1">
+        <v>11723</v>
+      </c>
+      <c r="BG26" s="1">
+        <v>14882</v>
+      </c>
+      <c r="BH26" s="1">
+        <v>14635</v>
+      </c>
+      <c r="BI26" s="1">
+        <v>15719</v>
+      </c>
+    </row>
+    <row r="27" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V27" s="1">
+        <v>1577</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1476</v>
+      </c>
+      <c r="X27" s="1">
+        <v>2036</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>2075</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>521</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>267</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>2025</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>2676</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>2637</v>
+      </c>
+      <c r="AF27" s="1">
+        <v>6314</v>
+      </c>
+      <c r="AG27" s="1">
+        <v>2792</v>
+      </c>
+      <c r="AH27" s="1">
+        <v>4331</v>
+      </c>
+      <c r="AI27" s="1">
+        <v>4805</v>
+      </c>
+      <c r="AJ27" s="1">
+        <v>4946</v>
+      </c>
+      <c r="AK27" s="1">
+        <v>6151</v>
+      </c>
+      <c r="AL27" s="1">
+        <v>5393</v>
+      </c>
+      <c r="AM27" s="1">
+        <v>6796</v>
+      </c>
+      <c r="AN27" s="1">
+        <v>4884</v>
+      </c>
+      <c r="AO27" s="1">
+        <v>5531</v>
+      </c>
+      <c r="AP27" s="1">
+        <v>4579</v>
+      </c>
+      <c r="AQ27" s="1">
+        <v>3206</v>
+      </c>
+      <c r="AR27" s="1">
+        <v>3235</v>
+      </c>
+      <c r="AS27" s="1">
+        <v>3340</v>
+      </c>
+      <c r="AT27" s="1">
+        <v>3664</v>
+      </c>
+      <c r="AU27" s="1">
+        <v>4276</v>
+      </c>
+      <c r="AV27" s="1">
+        <v>4564</v>
+      </c>
+      <c r="AW27" s="1">
+        <v>3306</v>
+      </c>
+      <c r="AX27" s="1">
+        <v>3272</v>
+      </c>
+      <c r="AY27" s="1">
+        <v>6415</v>
+      </c>
+      <c r="AZ27" s="1">
+        <v>8656</v>
+      </c>
+      <c r="BA27" s="1">
+        <v>8686</v>
+      </c>
+      <c r="BB27" s="1">
+        <v>10905</v>
+      </c>
+      <c r="BC27" s="1">
+        <v>9473</v>
+      </c>
+      <c r="BD27" s="1">
+        <v>9026</v>
+      </c>
+      <c r="BE27" s="1">
+        <v>11624</v>
+      </c>
+      <c r="BF27" s="1">
+        <v>10360</v>
+      </c>
+      <c r="BG27" s="1">
+        <v>13829</v>
+      </c>
+      <c r="BH27" s="1">
+        <v>13583</v>
+      </c>
+      <c r="BI27" s="1">
+        <v>14667</v>
+      </c>
+    </row>
+    <row r="28" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V28" s="1">
+        <v>4389</v>
+      </c>
+      <c r="W28" s="1">
+        <v>4288</v>
+      </c>
+      <c r="X28" s="1">
+        <v>4848</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>4887</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>3333</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>5433</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>1757</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>2408</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>2370</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>6047</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>2525</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>4064</v>
+      </c>
+      <c r="AI28" s="1">
+        <v>4537</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>4679</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>5884</v>
+      </c>
+      <c r="AL28" s="1">
+        <v>5126</v>
+      </c>
+      <c r="AM28" s="1">
+        <v>6529</v>
+      </c>
+      <c r="AN28" s="1">
+        <v>4637</v>
+      </c>
+      <c r="AO28" s="1">
+        <v>6163</v>
+      </c>
+      <c r="AP28" s="1">
+        <v>4382</v>
+      </c>
+      <c r="AQ28" s="1">
+        <v>4956</v>
+      </c>
+      <c r="AR28" s="1">
+        <v>5009</v>
+      </c>
+      <c r="AS28" s="1">
+        <v>5114</v>
+      </c>
+      <c r="AT28" s="1">
+        <v>4288</v>
+      </c>
+      <c r="AU28" s="1">
+        <v>4009</v>
+      </c>
+      <c r="AV28" s="1">
+        <v>4297</v>
+      </c>
+      <c r="AW28" s="1">
+        <v>4726</v>
+      </c>
+      <c r="AX28" s="1">
+        <v>5475</v>
+      </c>
+      <c r="AY28" s="1">
+        <v>8382</v>
+      </c>
+      <c r="AZ28" s="1">
+        <v>10622</v>
+      </c>
+      <c r="BA28" s="1">
+        <v>10653</v>
+      </c>
+      <c r="BB28" s="1">
+        <v>12870</v>
+      </c>
+      <c r="BC28" s="1">
+        <v>11410</v>
+      </c>
+      <c r="BD28" s="1">
+        <v>10992</v>
+      </c>
+      <c r="BE28" s="1">
+        <v>13589</v>
+      </c>
+      <c r="BF28" s="1">
+        <v>15520</v>
+      </c>
+      <c r="BG28" s="1">
+        <v>15368</v>
+      </c>
+      <c r="BH28" s="1">
+        <v>15121</v>
+      </c>
+      <c r="BI28" s="1">
+        <v>16205</v>
+      </c>
+    </row>
+    <row r="29" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V29" s="1">
+        <v>2748</v>
+      </c>
+      <c r="W29" s="1">
+        <v>2647</v>
+      </c>
+      <c r="X29" s="1">
+        <v>3207</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>3245</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>1692</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>3792</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>1436</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>1621</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>1582</v>
+      </c>
+      <c r="AF29" s="1">
+        <v>5259</v>
+      </c>
+      <c r="AG29" s="1">
+        <v>1737</v>
+      </c>
+      <c r="AH29" s="1">
+        <v>3276</v>
+      </c>
+      <c r="AI29" s="1">
+        <v>3750</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>3891</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>5096</v>
+      </c>
+      <c r="AL29" s="1">
+        <v>4338</v>
+      </c>
+      <c r="AM29" s="1">
+        <v>5741</v>
+      </c>
+      <c r="AN29" s="1">
+        <v>3848</v>
+      </c>
+      <c r="AO29" s="1">
+        <v>4495</v>
+      </c>
+      <c r="AP29" s="1">
+        <v>3593</v>
+      </c>
+      <c r="AQ29" s="1">
+        <v>4167</v>
+      </c>
+      <c r="AR29" s="1">
+        <v>5449</v>
+      </c>
+      <c r="AS29" s="1">
+        <v>5554</v>
+      </c>
+      <c r="AT29" s="1">
+        <v>3498</v>
+      </c>
+      <c r="AU29" s="1">
+        <v>3220</v>
+      </c>
+      <c r="AV29" s="1">
+        <v>3508</v>
+      </c>
+      <c r="AW29" s="1">
+        <v>3937</v>
+      </c>
+      <c r="AX29" s="1">
+        <v>4686</v>
+      </c>
+      <c r="AY29" s="1">
+        <v>10393</v>
+      </c>
+      <c r="AZ29" s="1">
+        <v>11710</v>
+      </c>
+      <c r="BA29" s="1">
+        <v>11741</v>
+      </c>
+      <c r="BB29" s="1">
+        <v>9497</v>
+      </c>
+      <c r="BC29" s="1">
+        <v>12527</v>
+      </c>
+      <c r="BD29" s="1">
+        <v>12081</v>
+      </c>
+      <c r="BE29" s="1">
+        <v>15600</v>
+      </c>
+      <c r="BF29" s="1">
+        <v>14731</v>
+      </c>
+      <c r="BG29" s="1">
+        <v>14579</v>
+      </c>
+      <c r="BH29" s="1">
+        <v>14332</v>
+      </c>
+      <c r="BI29" s="1">
+        <v>15416</v>
+      </c>
+    </row>
+    <row r="30" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V30" s="1">
+        <v>4527</v>
+      </c>
+      <c r="W30" s="1">
+        <v>4425</v>
+      </c>
+      <c r="X30" s="1">
+        <v>4986</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>5024</v>
+      </c>
+      <c r="Z30" s="1">
+        <v>3471</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>5571</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>3215</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>1895</v>
+      </c>
+      <c r="AD30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="1">
+        <v>2062</v>
+      </c>
+      <c r="AF30" s="1">
+        <v>3568</v>
+      </c>
+      <c r="AG30" s="1">
+        <v>2217</v>
+      </c>
+      <c r="AH30" s="1">
+        <v>3756</v>
+      </c>
+      <c r="AI30" s="1">
+        <v>4230</v>
+      </c>
+      <c r="AJ30" s="1">
+        <v>4372</v>
+      </c>
+      <c r="AK30" s="1">
+        <v>5730</v>
+      </c>
+      <c r="AL30" s="1">
+        <v>4818</v>
+      </c>
+      <c r="AM30" s="1">
+        <v>4881</v>
+      </c>
+      <c r="AN30" s="1">
+        <v>3298</v>
+      </c>
+      <c r="AO30" s="1">
+        <v>2928</v>
+      </c>
+      <c r="AP30" s="1">
+        <v>3043</v>
+      </c>
+      <c r="AQ30" s="1">
+        <v>3617</v>
+      </c>
+      <c r="AR30" s="1">
+        <v>4900</v>
+      </c>
+      <c r="AS30" s="1">
+        <v>5005</v>
+      </c>
+      <c r="AT30" s="1">
+        <v>2949</v>
+      </c>
+      <c r="AU30" s="1">
+        <v>2670</v>
+      </c>
+      <c r="AV30" s="1">
+        <v>2958</v>
+      </c>
+      <c r="AW30" s="1">
+        <v>3387</v>
+      </c>
+      <c r="AX30" s="1">
+        <v>4136</v>
+      </c>
+      <c r="AY30" s="1">
+        <v>9844</v>
+      </c>
+      <c r="AZ30" s="1">
+        <v>9787</v>
+      </c>
+      <c r="BA30" s="1">
+        <v>9818</v>
+      </c>
+      <c r="BB30" s="1">
+        <v>14332</v>
+      </c>
+      <c r="BC30" s="1">
+        <v>12872</v>
+      </c>
+      <c r="BD30" s="1">
+        <v>12454</v>
+      </c>
+      <c r="BE30" s="1">
+        <v>15051</v>
+      </c>
+      <c r="BF30" s="1">
+        <v>14181</v>
+      </c>
+      <c r="BG30" s="1">
+        <v>14029</v>
+      </c>
+      <c r="BH30" s="1">
+        <v>13783</v>
+      </c>
+      <c r="BI30" s="1">
+        <v>14867</v>
+      </c>
+    </row>
+    <row r="31" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V31" s="1">
+        <v>7754</v>
+      </c>
+      <c r="W31" s="1">
+        <v>7652</v>
+      </c>
+      <c r="X31" s="1">
+        <v>8213</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>8251</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>6698</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>8797</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>6442</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>5122</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>191</v>
+      </c>
+      <c r="AE31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="1">
+        <v>3740</v>
+      </c>
+      <c r="AG31" s="1">
+        <v>156</v>
+      </c>
+      <c r="AH31" s="1">
+        <v>1757</v>
+      </c>
+      <c r="AI31" s="1">
+        <v>2231</v>
+      </c>
+      <c r="AJ31" s="1">
+        <v>2372</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>3577</v>
+      </c>
+      <c r="AL31" s="1">
+        <v>2819</v>
+      </c>
+      <c r="AM31" s="1">
+        <v>4222</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>4834</v>
+      </c>
+      <c r="AO31" s="1">
+        <v>3857</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>3234</v>
+      </c>
+      <c r="AQ31" s="1">
+        <v>3808</v>
+      </c>
+      <c r="AR31" s="1">
+        <v>5091</v>
+      </c>
+      <c r="AS31" s="1">
+        <v>5196</v>
+      </c>
+      <c r="AT31" s="1">
+        <v>3140</v>
+      </c>
+      <c r="AU31" s="1">
+        <v>2861</v>
+      </c>
+      <c r="AV31" s="1">
+        <v>3149</v>
+      </c>
+      <c r="AW31" s="1">
+        <v>3578</v>
+      </c>
+      <c r="AX31" s="1">
+        <v>4327</v>
+      </c>
+      <c r="AY31" s="1">
+        <v>12842</v>
+      </c>
+      <c r="AZ31" s="1">
+        <v>13762</v>
+      </c>
+      <c r="BA31" s="1">
+        <v>13792</v>
+      </c>
+      <c r="BB31" s="1">
+        <v>17325</v>
+      </c>
+      <c r="BC31" s="1">
+        <v>15866</v>
+      </c>
+      <c r="BD31" s="1">
+        <v>15515</v>
+      </c>
+      <c r="BE31" s="1">
+        <v>18044</v>
+      </c>
+      <c r="BF31" s="1">
+        <v>18156</v>
+      </c>
+      <c r="BG31" s="1">
+        <v>18027</v>
+      </c>
+      <c r="BH31" s="1">
+        <v>17781</v>
+      </c>
+      <c r="BI31" s="1">
+        <v>18841</v>
+      </c>
+    </row>
+    <row r="32" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="V32" s="1">
+        <v>4014</v>
+      </c>
+      <c r="W32" s="1">
+        <v>3912</v>
+      </c>
+      <c r="X32" s="1">
+        <v>4473</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>4511</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>2958</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>5058</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>2702</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>1382</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>1273</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>1234</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="1">
+        <v>1389</v>
+      </c>
+      <c r="AH32" s="1">
+        <v>2928</v>
+      </c>
+      <c r="AI32" s="1">
+        <v>3402</v>
+      </c>
+      <c r="AJ32" s="1">
+        <v>3543</v>
+      </c>
+      <c r="AK32" s="1">
+        <v>4748</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>3990</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>5393</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>3939</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>5028</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>3684</v>
+      </c>
+      <c r="AQ32" s="1">
+        <v>4258</v>
+      </c>
+      <c r="AR32" s="1">
+        <v>5540</v>
+      </c>
+      <c r="AS32" s="1">
+        <v>5645</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>3589</v>
+      </c>
+      <c r="AU32" s="1">
+        <v>3310</v>
+      </c>
+      <c r="AV32" s="1">
+        <v>3599</v>
+      </c>
+      <c r="AW32" s="1">
+        <v>4027</v>
+      </c>
+      <c r="AX32" s="1">
+        <v>4777</v>
+      </c>
+      <c r="AY32" s="1">
+        <v>10484</v>
+      </c>
+      <c r="AZ32" s="1">
+        <v>10428</v>
+      </c>
+      <c r="BA32" s="1">
+        <v>10458</v>
+      </c>
+      <c r="BB32" s="1">
+        <v>14972</v>
+      </c>
+      <c r="BC32" s="1">
+        <v>13513</v>
+      </c>
+      <c r="BD32" s="1">
+        <v>13095</v>
+      </c>
+      <c r="BE32" s="1">
+        <v>15691</v>
+      </c>
+      <c r="BF32" s="1">
+        <v>14822</v>
+      </c>
+      <c r="BG32" s="1">
+        <v>14669</v>
+      </c>
+      <c r="BH32" s="1">
+        <v>14423</v>
+      </c>
+      <c r="BI32" s="1">
+        <v>15507</v>
+      </c>
+    </row>
+    <row r="33" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V33" s="1">
+        <v>7596</v>
+      </c>
+      <c r="W33" s="1">
+        <v>7494</v>
+      </c>
+      <c r="X33" s="1">
+        <v>8055</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>8093</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>6540</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>8640</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>6284</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>4964</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>305</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>201</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>3582</v>
+      </c>
+      <c r="AG33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="1">
+        <v>1599</v>
+      </c>
+      <c r="AI33" s="1">
+        <v>2073</v>
+      </c>
+      <c r="AJ33" s="1">
+        <v>2215</v>
+      </c>
+      <c r="AK33" s="1">
+        <v>3420</v>
+      </c>
+      <c r="AL33" s="1">
+        <v>2661</v>
+      </c>
+      <c r="AM33" s="1">
+        <v>4064</v>
+      </c>
+      <c r="AN33" s="1">
+        <v>4676</v>
+      </c>
+      <c r="AO33" s="1">
+        <v>3699</v>
+      </c>
+      <c r="AP33" s="1">
+        <v>3349</v>
+      </c>
+      <c r="AQ33" s="1">
+        <v>3923</v>
+      </c>
+      <c r="AR33" s="1">
+        <v>5205</v>
+      </c>
+      <c r="AS33" s="1">
+        <v>5310</v>
+      </c>
+      <c r="AT33" s="1">
+        <v>3254</v>
+      </c>
+      <c r="AU33" s="1">
+        <v>2975</v>
+      </c>
+      <c r="AV33" s="1">
+        <v>3264</v>
+      </c>
+      <c r="AW33" s="1">
+        <v>3692</v>
+      </c>
+      <c r="AX33" s="1">
+        <v>4442</v>
+      </c>
+      <c r="AY33" s="1">
+        <v>12684</v>
+      </c>
+      <c r="AZ33" s="1">
+        <v>13604</v>
+      </c>
+      <c r="BA33" s="1">
+        <v>13635</v>
+      </c>
+      <c r="BB33" s="1">
+        <v>17167</v>
+      </c>
+      <c r="BC33" s="1">
+        <v>15708</v>
+      </c>
+      <c r="BD33" s="1">
+        <v>15358</v>
+      </c>
+      <c r="BE33" s="1">
+        <v>17886</v>
+      </c>
+      <c r="BF33" s="1">
+        <v>17998</v>
+      </c>
+      <c r="BG33" s="1">
+        <v>17869</v>
+      </c>
+      <c r="BH33" s="1">
+        <v>17623</v>
+      </c>
+      <c r="BI33" s="1">
+        <v>18683</v>
+      </c>
+    </row>
+    <row r="34" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V34" s="1">
+        <v>5997</v>
+      </c>
+      <c r="W34" s="1">
+        <v>5895</v>
+      </c>
+      <c r="X34" s="1">
+        <v>6456</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>6494</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>4941</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>7040</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>4685</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>3365</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>3255</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>3217</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>1983</v>
+      </c>
+      <c r="AG34" s="1">
+        <v>3372</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="1">
+        <v>474</v>
+      </c>
+      <c r="AJ34" s="1">
+        <v>615</v>
+      </c>
+      <c r="AK34" s="1">
+        <v>1821</v>
+      </c>
+      <c r="AL34" s="1">
+        <v>1062</v>
+      </c>
+      <c r="AM34" s="1">
+        <v>2465</v>
+      </c>
+      <c r="AN34" s="1">
+        <v>3077</v>
+      </c>
+      <c r="AO34" s="1">
+        <v>2100</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>2986</v>
+      </c>
+      <c r="AQ34" s="1">
+        <v>3560</v>
+      </c>
+      <c r="AR34" s="1">
+        <v>7719</v>
+      </c>
+      <c r="AS34" s="1">
+        <v>7824</v>
+      </c>
+      <c r="AT34" s="1">
+        <v>2892</v>
+      </c>
+      <c r="AU34" s="1">
+        <v>2613</v>
+      </c>
+      <c r="AV34" s="1">
+        <v>2901</v>
+      </c>
+      <c r="AW34" s="1">
+        <v>3330</v>
+      </c>
+      <c r="AX34" s="1">
+        <v>4079</v>
+      </c>
+      <c r="AY34" s="1">
+        <v>11085</v>
+      </c>
+      <c r="AZ34" s="1">
+        <v>12005</v>
+      </c>
+      <c r="BA34" s="1">
+        <v>12036</v>
+      </c>
+      <c r="BB34" s="1">
+        <v>15568</v>
+      </c>
+      <c r="BC34" s="1">
+        <v>14109</v>
+      </c>
+      <c r="BD34" s="1">
+        <v>13759</v>
+      </c>
+      <c r="BE34" s="1">
+        <v>16287</v>
+      </c>
+      <c r="BF34" s="1">
+        <v>16399</v>
+      </c>
+      <c r="BG34" s="1">
+        <v>16270</v>
+      </c>
+      <c r="BH34" s="1">
+        <v>16024</v>
+      </c>
+      <c r="BI34" s="1">
+        <v>17084</v>
+      </c>
+    </row>
+    <row r="35" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V35" s="1">
+        <v>8226</v>
+      </c>
+      <c r="W35" s="1">
+        <v>8125</v>
+      </c>
+      <c r="X35" s="1">
+        <v>7401</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>7638</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>7170</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>6857</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>7124</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>5594</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>6048</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>6009</v>
+      </c>
+      <c r="AF35" s="1">
+        <v>4212</v>
+      </c>
+      <c r="AG35" s="1">
+        <v>6164</v>
+      </c>
+      <c r="AH35" s="1">
+        <v>7703</v>
+      </c>
+      <c r="AI35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="1">
+        <v>197</v>
+      </c>
+      <c r="AK35" s="1">
+        <v>1454</v>
+      </c>
+      <c r="AL35" s="1">
+        <v>696</v>
+      </c>
+      <c r="AM35" s="1">
+        <v>2099</v>
+      </c>
+      <c r="AN35" s="1">
+        <v>2711</v>
+      </c>
+      <c r="AO35" s="1">
+        <v>4310</v>
+      </c>
+      <c r="AP35" s="1">
+        <v>4126</v>
+      </c>
+      <c r="AQ35" s="1">
+        <v>4503</v>
+      </c>
+      <c r="AR35" s="1">
+        <v>7353</v>
+      </c>
+      <c r="AS35" s="1">
+        <v>7458</v>
+      </c>
+      <c r="AT35" s="1">
+        <v>3835</v>
+      </c>
+      <c r="AU35" s="1">
+        <v>3556</v>
+      </c>
+      <c r="AV35" s="1">
+        <v>3844</v>
+      </c>
+      <c r="AW35" s="1">
+        <v>4273</v>
+      </c>
+      <c r="AX35" s="1">
+        <v>5022</v>
+      </c>
+      <c r="AY35" s="1">
+        <v>10719</v>
+      </c>
+      <c r="AZ35" s="1">
+        <v>11639</v>
+      </c>
+      <c r="BA35" s="1">
+        <v>11669</v>
+      </c>
+      <c r="BB35" s="1">
+        <v>15202</v>
+      </c>
+      <c r="BC35" s="1">
+        <v>13743</v>
+      </c>
+      <c r="BD35" s="1">
+        <v>13392</v>
+      </c>
+      <c r="BE35" s="1">
+        <v>15921</v>
+      </c>
+      <c r="BF35" s="1">
+        <v>16032</v>
+      </c>
+      <c r="BG35" s="1">
+        <v>15904</v>
+      </c>
+      <c r="BH35" s="1">
+        <v>15658</v>
+      </c>
+      <c r="BI35" s="1">
+        <v>16718</v>
+      </c>
+    </row>
+    <row r="36" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V36" s="1">
+        <v>8039</v>
+      </c>
+      <c r="W36" s="1">
+        <v>7938</v>
+      </c>
+      <c r="X36" s="1">
+        <v>7214</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>7451</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>6983</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>6670</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>6937</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>5407</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>5860</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>5822</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>4025</v>
+      </c>
+      <c r="AG36" s="1">
+        <v>5977</v>
+      </c>
+      <c r="AH36" s="1">
+        <v>7516</v>
+      </c>
+      <c r="AI36" s="1">
+        <v>197</v>
+      </c>
+      <c r="AJ36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="1">
+        <v>1267</v>
+      </c>
+      <c r="AL36" s="1">
+        <v>509</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>1912</v>
+      </c>
+      <c r="AN36" s="1">
+        <v>2524</v>
+      </c>
+      <c r="AO36" s="1">
+        <v>4123</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>3939</v>
+      </c>
+      <c r="AQ36" s="1">
+        <v>4316</v>
+      </c>
+      <c r="AR36" s="1">
+        <v>7166</v>
+      </c>
+      <c r="AS36" s="1">
+        <v>7271</v>
+      </c>
+      <c r="AT36" s="1">
+        <v>3648</v>
+      </c>
+      <c r="AU36" s="1">
+        <v>3369</v>
+      </c>
+      <c r="AV36" s="1">
+        <v>3657</v>
+      </c>
+      <c r="AW36" s="1">
+        <v>4086</v>
+      </c>
+      <c r="AX36" s="1">
+        <v>4835</v>
+      </c>
+      <c r="AY36" s="1">
+        <v>10532</v>
+      </c>
+      <c r="AZ36" s="1">
+        <v>11451</v>
+      </c>
+      <c r="BA36" s="1">
+        <v>11482</v>
+      </c>
+      <c r="BB36" s="1">
+        <v>15015</v>
+      </c>
+      <c r="BC36" s="1">
+        <v>13555</v>
+      </c>
+      <c r="BD36" s="1">
+        <v>13205</v>
+      </c>
+      <c r="BE36" s="1">
+        <v>15734</v>
+      </c>
+      <c r="BF36" s="1">
+        <v>15845</v>
+      </c>
+      <c r="BG36" s="1">
+        <v>15717</v>
+      </c>
+      <c r="BH36" s="1">
+        <v>15470</v>
+      </c>
+      <c r="BI36" s="1">
+        <v>16531</v>
+      </c>
+    </row>
+    <row r="37" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V37" s="1">
+        <v>6844</v>
+      </c>
+      <c r="W37" s="1">
+        <v>6743</v>
+      </c>
+      <c r="X37" s="1">
+        <v>7303</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>7342</v>
+      </c>
+      <c r="Z37" s="1">
+        <v>5788</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>7888</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>5533</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>4212</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>4103</v>
+      </c>
+      <c r="AE37" s="1">
+        <v>4064</v>
+      </c>
+      <c r="AF37" s="1">
+        <v>2830</v>
+      </c>
+      <c r="AG37" s="1">
+        <v>4219</v>
+      </c>
+      <c r="AH37" s="1">
+        <v>5758</v>
+      </c>
+      <c r="AI37" s="1">
+        <v>6232</v>
+      </c>
+      <c r="AJ37" s="1">
+        <v>6374</v>
+      </c>
+      <c r="AK37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="1">
+        <v>6820</v>
+      </c>
+      <c r="AM37" s="1">
+        <v>7024</v>
+      </c>
+      <c r="AN37" s="1">
+        <v>4786</v>
+      </c>
+      <c r="AO37" s="1">
+        <v>3644</v>
+      </c>
+      <c r="AP37" s="1">
+        <v>4531</v>
+      </c>
+      <c r="AQ37" s="1">
+        <v>5105</v>
+      </c>
+      <c r="AR37" s="1">
+        <v>6387</v>
+      </c>
+      <c r="AS37" s="1">
+        <v>6492</v>
+      </c>
+      <c r="AT37" s="1">
+        <v>4436</v>
+      </c>
+      <c r="AU37" s="1">
+        <v>4157</v>
+      </c>
+      <c r="AV37" s="1">
+        <v>4446</v>
+      </c>
+      <c r="AW37" s="1">
+        <v>4874</v>
+      </c>
+      <c r="AX37" s="1">
+        <v>5624</v>
+      </c>
+      <c r="AY37" s="1">
+        <v>11331</v>
+      </c>
+      <c r="AZ37" s="1">
+        <v>11275</v>
+      </c>
+      <c r="BA37" s="1">
+        <v>11305</v>
+      </c>
+      <c r="BB37" s="1">
+        <v>15819</v>
+      </c>
+      <c r="BC37" s="1">
+        <v>14360</v>
+      </c>
+      <c r="BD37" s="1">
+        <v>13942</v>
+      </c>
+      <c r="BE37" s="1">
+        <v>16538</v>
+      </c>
+      <c r="BF37" s="1">
+        <v>15669</v>
+      </c>
+      <c r="BG37" s="1">
+        <v>15517</v>
+      </c>
+      <c r="BH37" s="1">
+        <v>15270</v>
+      </c>
+      <c r="BI37" s="1">
+        <v>16354</v>
+      </c>
+    </row>
+    <row r="38" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V38" s="1">
+        <v>7531</v>
+      </c>
+      <c r="W38" s="1">
+        <v>7429</v>
+      </c>
+      <c r="X38" s="1">
+        <v>6705</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>6942</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>6474</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>6162</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>6429</v>
+      </c>
+      <c r="AC38" s="1">
+        <v>4899</v>
+      </c>
+      <c r="AD38" s="1">
+        <v>5352</v>
+      </c>
+      <c r="AE38" s="1">
+        <v>5313</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>3517</v>
+      </c>
+      <c r="AG38" s="1">
+        <v>5468</v>
+      </c>
+      <c r="AH38" s="1">
+        <v>7007</v>
+      </c>
+      <c r="AI38" s="1">
+        <v>2502</v>
+      </c>
+      <c r="AJ38" s="1">
+        <v>2643</v>
+      </c>
+      <c r="AK38" s="1">
+        <v>759</v>
+      </c>
+      <c r="AL38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>1403</v>
+      </c>
+      <c r="AN38" s="1">
+        <v>2015</v>
+      </c>
+      <c r="AO38" s="1">
+        <v>3615</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>3431</v>
+      </c>
+      <c r="AQ38" s="1">
+        <v>3808</v>
+      </c>
+      <c r="AR38" s="1">
+        <v>6657</v>
+      </c>
+      <c r="AS38" s="1">
+        <v>6762</v>
+      </c>
+      <c r="AT38" s="1">
+        <v>3139</v>
+      </c>
+      <c r="AU38" s="1">
+        <v>2861</v>
+      </c>
+      <c r="AV38" s="1">
+        <v>3149</v>
+      </c>
+      <c r="AW38" s="1">
+        <v>3577</v>
+      </c>
+      <c r="AX38" s="1">
+        <v>4327</v>
+      </c>
+      <c r="AY38" s="1">
+        <v>10023</v>
+      </c>
+      <c r="AZ38" s="1">
+        <v>10943</v>
+      </c>
+      <c r="BA38" s="1">
+        <v>10974</v>
+      </c>
+      <c r="BB38" s="1">
+        <v>14506</v>
+      </c>
+      <c r="BC38" s="1">
+        <v>13047</v>
+      </c>
+      <c r="BD38" s="1">
+        <v>12697</v>
+      </c>
+      <c r="BE38" s="1">
+        <v>15225</v>
+      </c>
+      <c r="BF38" s="1">
+        <v>15337</v>
+      </c>
+      <c r="BG38" s="1">
+        <v>15208</v>
+      </c>
+      <c r="BH38" s="1">
+        <v>14962</v>
+      </c>
+      <c r="BI38" s="1">
+        <v>16022</v>
+      </c>
+    </row>
+    <row r="39" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V39" s="1">
+        <v>9268</v>
+      </c>
+      <c r="W39" s="1">
+        <v>9166</v>
+      </c>
+      <c r="X39" s="1">
+        <v>8859</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>9765</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>8211</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>8315</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>7956</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>6636</v>
+      </c>
+      <c r="AD39" s="1">
+        <v>6526</v>
+      </c>
+      <c r="AE39" s="1">
+        <v>6488</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>5254</v>
+      </c>
+      <c r="AG39" s="1">
+        <v>6643</v>
+      </c>
+      <c r="AH39" s="1">
+        <v>8182</v>
+      </c>
+      <c r="AI39" s="1">
+        <v>4655</v>
+      </c>
+      <c r="AJ39" s="1">
+        <v>4797</v>
+      </c>
+      <c r="AK39" s="1">
+        <v>2496</v>
+      </c>
+      <c r="AL39" s="1">
+        <v>5243</v>
+      </c>
+      <c r="AM39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="1">
+        <v>4169</v>
+      </c>
+      <c r="AO39" s="1">
+        <v>5768</v>
+      </c>
+      <c r="AP39" s="1">
+        <v>5584</v>
+      </c>
+      <c r="AQ39" s="1">
+        <v>5961</v>
+      </c>
+      <c r="AR39" s="1">
+        <v>8811</v>
+      </c>
+      <c r="AS39" s="1">
+        <v>8916</v>
+      </c>
+      <c r="AT39" s="1">
+        <v>5293</v>
+      </c>
+      <c r="AU39" s="1">
+        <v>5014</v>
+      </c>
+      <c r="AV39" s="1">
+        <v>5302</v>
+      </c>
+      <c r="AW39" s="1">
+        <v>5731</v>
+      </c>
+      <c r="AX39" s="1">
+        <v>6480</v>
+      </c>
+      <c r="AY39" s="1">
+        <v>9602</v>
+      </c>
+      <c r="AZ39" s="1">
+        <v>8577</v>
+      </c>
+      <c r="BA39" s="1">
+        <v>8607</v>
+      </c>
+      <c r="BB39" s="1">
+        <v>15683</v>
+      </c>
+      <c r="BC39" s="1">
+        <v>11448</v>
+      </c>
+      <c r="BD39" s="1">
+        <v>11001</v>
+      </c>
+      <c r="BE39" s="1">
+        <v>13201</v>
+      </c>
+      <c r="BF39" s="1">
+        <v>12971</v>
+      </c>
+      <c r="BG39" s="1">
+        <v>12819</v>
+      </c>
+      <c r="BH39" s="1">
+        <v>12572</v>
+      </c>
+      <c r="BI39" s="1">
+        <v>13656</v>
+      </c>
+    </row>
+    <row r="40" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V40" s="1">
+        <v>6041</v>
+      </c>
+      <c r="W40" s="1">
+        <v>5939</v>
+      </c>
+      <c r="X40" s="1">
+        <v>5419</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>5656</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>4985</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>4876</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>4729</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>3409</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>3615</v>
+      </c>
+      <c r="AE40" s="1">
+        <v>3576</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>5081</v>
+      </c>
+      <c r="AG40" s="1">
+        <v>3731</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>5270</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>2425</v>
+      </c>
+      <c r="AJ40" s="1">
+        <v>2566</v>
+      </c>
+      <c r="AK40" s="1">
+        <v>3739</v>
+      </c>
+      <c r="AL40" s="1">
+        <v>3013</v>
+      </c>
+      <c r="AM40" s="1">
+        <v>2890</v>
+      </c>
+      <c r="AN40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="1">
+        <v>1878</v>
+      </c>
+      <c r="AP40" s="1">
+        <v>2151</v>
+      </c>
+      <c r="AQ40" s="1">
+        <v>2734</v>
+      </c>
+      <c r="AR40" s="1">
+        <v>5371</v>
+      </c>
+      <c r="AS40" s="1">
+        <v>5476</v>
+      </c>
+      <c r="AT40" s="1">
+        <v>2066</v>
+      </c>
+      <c r="AU40" s="1">
+        <v>1787</v>
+      </c>
+      <c r="AV40" s="1">
+        <v>2075</v>
+      </c>
+      <c r="AW40" s="1">
+        <v>2504</v>
+      </c>
+      <c r="AX40" s="1">
+        <v>3253</v>
+      </c>
+      <c r="AY40" s="1">
+        <v>8732</v>
+      </c>
+      <c r="AZ40" s="1">
+        <v>10972</v>
+      </c>
+      <c r="BA40" s="1">
+        <v>11003</v>
+      </c>
+      <c r="BB40" s="1">
+        <v>13218</v>
+      </c>
+      <c r="BC40" s="1">
+        <v>11758</v>
+      </c>
+      <c r="BD40" s="1">
+        <v>11408</v>
+      </c>
+      <c r="BE40" s="1">
+        <v>13937</v>
+      </c>
+      <c r="BF40" s="1">
+        <v>16300</v>
+      </c>
+      <c r="BG40" s="1">
+        <v>16148</v>
+      </c>
+      <c r="BH40" s="1">
+        <v>15902</v>
+      </c>
+      <c r="BI40" s="1">
+        <v>16986</v>
+      </c>
+    </row>
+    <row r="41" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V41" s="1">
+        <v>5394</v>
+      </c>
+      <c r="W41" s="1">
+        <v>5292</v>
+      </c>
+      <c r="X41" s="1">
+        <v>5853</v>
+      </c>
+      <c r="Y41" s="1">
+        <v>5891</v>
+      </c>
+      <c r="Z41" s="1">
+        <v>4337</v>
+      </c>
+      <c r="AA41" s="1">
+        <v>4418</v>
+      </c>
+      <c r="AB41" s="1">
+        <v>4082</v>
+      </c>
+      <c r="AC41" s="1">
+        <v>2762</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>2968</v>
+      </c>
+      <c r="AE41" s="1">
+        <v>2929</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>4434</v>
+      </c>
+      <c r="AG41" s="1">
+        <v>3084</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>4623</v>
+      </c>
+      <c r="AI41" s="1">
+        <v>2932</v>
+      </c>
+      <c r="AJ41" s="1">
+        <v>3074</v>
+      </c>
+      <c r="AK41" s="1">
+        <v>4170</v>
+      </c>
+      <c r="AL41" s="1">
+        <v>3520</v>
+      </c>
+      <c r="AM41" s="1">
+        <v>3322</v>
+      </c>
+      <c r="AN41" s="1">
+        <v>1738</v>
+      </c>
+      <c r="AO41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP41" s="1">
+        <v>1483</v>
+      </c>
+      <c r="AQ41" s="1">
+        <v>2057</v>
+      </c>
+      <c r="AR41" s="1">
+        <v>3340</v>
+      </c>
+      <c r="AS41" s="1">
+        <v>3445</v>
+      </c>
+      <c r="AT41" s="1">
+        <v>1389</v>
+      </c>
+      <c r="AU41" s="1">
+        <v>1110</v>
+      </c>
+      <c r="AV41" s="1">
+        <v>1398</v>
+      </c>
+      <c r="AW41" s="1">
+        <v>1827</v>
+      </c>
+      <c r="AX41" s="1">
+        <v>2576</v>
+      </c>
+      <c r="AY41" s="1">
+        <v>8284</v>
+      </c>
+      <c r="AZ41" s="1">
+        <v>8227</v>
+      </c>
+      <c r="BA41" s="1">
+        <v>8258</v>
+      </c>
+      <c r="BB41" s="1">
+        <v>12772</v>
+      </c>
+      <c r="BC41" s="1">
+        <v>11312</v>
+      </c>
+      <c r="BD41" s="1">
+        <v>10894</v>
+      </c>
+      <c r="BE41" s="1">
+        <v>13491</v>
+      </c>
+      <c r="BF41" s="1">
+        <v>12621</v>
+      </c>
+      <c r="BG41" s="1">
+        <v>12469</v>
+      </c>
+      <c r="BH41" s="1">
+        <v>12223</v>
+      </c>
+      <c r="BI41" s="1">
+        <v>13307</v>
+      </c>
+    </row>
+    <row r="42" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V42" s="1">
+        <v>4816</v>
+      </c>
+      <c r="W42" s="1">
+        <v>4679</v>
+      </c>
+      <c r="X42" s="1">
+        <v>3782</v>
+      </c>
+      <c r="Y42" s="1">
+        <v>4020</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>3760</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>3239</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>3506</v>
+      </c>
+      <c r="AC42" s="1">
+        <v>3640</v>
+      </c>
+      <c r="AD42" s="1">
+        <v>4291</v>
+      </c>
+      <c r="AE42" s="1">
+        <v>4252</v>
+      </c>
+      <c r="AF42" s="1">
+        <v>7929</v>
+      </c>
+      <c r="AG42" s="1">
+        <v>4407</v>
+      </c>
+      <c r="AH42" s="1">
+        <v>5946</v>
+      </c>
+      <c r="AI42" s="1">
+        <v>6577</v>
+      </c>
+      <c r="AJ42" s="1">
+        <v>6719</v>
+      </c>
+      <c r="AK42" s="1">
+        <v>7770</v>
+      </c>
+      <c r="AL42" s="1">
+        <v>7166</v>
+      </c>
+      <c r="AM42" s="1">
+        <v>6922</v>
+      </c>
+      <c r="AN42" s="1">
+        <v>5384</v>
+      </c>
+      <c r="AO42" s="1">
+        <v>6030</v>
+      </c>
+      <c r="AP42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ42" s="1">
+        <v>3705</v>
+      </c>
+      <c r="AR42" s="1">
+        <v>3735</v>
+      </c>
+      <c r="AS42" s="1">
+        <v>3839</v>
+      </c>
+      <c r="AT42" s="1">
+        <v>4164</v>
+      </c>
+      <c r="AU42" s="1">
+        <v>4642</v>
+      </c>
+      <c r="AV42" s="1">
+        <v>4930</v>
+      </c>
+      <c r="AW42" s="1">
+        <v>3806</v>
+      </c>
+      <c r="AX42" s="1">
+        <v>3771</v>
+      </c>
+      <c r="AY42" s="1">
+        <v>7104</v>
+      </c>
+      <c r="AZ42" s="1">
+        <v>9344</v>
+      </c>
+      <c r="BA42" s="1">
+        <v>9375</v>
+      </c>
+      <c r="BB42" s="1">
+        <v>11592</v>
+      </c>
+      <c r="BC42" s="1">
+        <v>10133</v>
+      </c>
+      <c r="BD42" s="1">
+        <v>9714</v>
+      </c>
+      <c r="BE42" s="1">
+        <v>12311</v>
+      </c>
+      <c r="BF42" s="1">
+        <v>11048</v>
+      </c>
+      <c r="BG42" s="1">
+        <v>14516</v>
+      </c>
+      <c r="BH42" s="1">
+        <v>14270</v>
+      </c>
+      <c r="BI42" s="1">
+        <v>15354</v>
+      </c>
+    </row>
+    <row r="43" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V43" s="1">
+        <v>6879</v>
+      </c>
+      <c r="W43" s="1">
+        <v>6777</v>
+      </c>
+      <c r="X43" s="1">
+        <v>5242</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>5480</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>5823</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>4699</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>4966</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>4247</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>4453</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>4414</v>
+      </c>
+      <c r="AF43" s="1">
+        <v>5919</v>
+      </c>
+      <c r="AG43" s="1">
+        <v>4569</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>6108</v>
+      </c>
+      <c r="AI43" s="1">
+        <v>3263</v>
+      </c>
+      <c r="AJ43" s="1">
+        <v>3404</v>
+      </c>
+      <c r="AK43" s="1">
+        <v>4458</v>
+      </c>
+      <c r="AL43" s="1">
+        <v>3851</v>
+      </c>
+      <c r="AM43" s="1">
+        <v>3609</v>
+      </c>
+      <c r="AN43" s="1">
+        <v>2069</v>
+      </c>
+      <c r="AO43" s="1">
+        <v>2716</v>
+      </c>
+      <c r="AP43" s="1">
+        <v>1764</v>
+      </c>
+      <c r="AQ43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR43" s="1">
+        <v>420</v>
+      </c>
+      <c r="AS43" s="1">
+        <v>525</v>
+      </c>
+      <c r="AT43" s="1">
+        <v>849</v>
+      </c>
+      <c r="AU43" s="1">
+        <v>1327</v>
+      </c>
+      <c r="AV43" s="1">
+        <v>1615</v>
+      </c>
+      <c r="AW43" s="1">
+        <v>438</v>
+      </c>
+      <c r="AX43" s="1">
+        <v>1590</v>
+      </c>
+      <c r="AY43" s="1">
+        <v>8564</v>
+      </c>
+      <c r="AZ43" s="1">
+        <v>7332</v>
+      </c>
+      <c r="BA43" s="1">
+        <v>7363</v>
+      </c>
+      <c r="BB43" s="1">
+        <v>13053</v>
+      </c>
+      <c r="BC43" s="1">
+        <v>11593</v>
+      </c>
+      <c r="BD43" s="1">
+        <v>11175</v>
+      </c>
+      <c r="BE43" s="1">
+        <v>13772</v>
+      </c>
+      <c r="BF43" s="1">
+        <v>11726</v>
+      </c>
+      <c r="BG43" s="1">
+        <v>11574</v>
+      </c>
+      <c r="BH43" s="1">
+        <v>11328</v>
+      </c>
+      <c r="BI43" s="1">
+        <v>12412</v>
+      </c>
+    </row>
+    <row r="44" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V44" s="1">
+        <v>6459</v>
+      </c>
+      <c r="W44" s="1">
+        <v>6357</v>
+      </c>
+      <c r="X44" s="1">
+        <v>4822</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>5060</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>5403</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>4279</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>4546</v>
+      </c>
+      <c r="AC44" s="1">
+        <v>3827</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>4033</v>
+      </c>
+      <c r="AE44" s="1">
+        <v>3994</v>
+      </c>
+      <c r="AF44" s="1">
+        <v>5499</v>
+      </c>
+      <c r="AG44" s="1">
+        <v>4149</v>
+      </c>
+      <c r="AH44" s="1">
+        <v>5688</v>
+      </c>
+      <c r="AI44" s="1">
+        <v>2843</v>
+      </c>
+      <c r="AJ44" s="1">
+        <v>2984</v>
+      </c>
+      <c r="AK44" s="1">
+        <v>4038</v>
+      </c>
+      <c r="AL44" s="1">
+        <v>3431</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>3190</v>
+      </c>
+      <c r="AN44" s="1">
+        <v>1649</v>
+      </c>
+      <c r="AO44" s="1">
+        <v>2296</v>
+      </c>
+      <c r="AP44" s="1">
+        <v>1344</v>
+      </c>
+      <c r="AQ44" s="1">
+        <v>1855</v>
+      </c>
+      <c r="AR44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="1">
+        <v>105</v>
+      </c>
+      <c r="AT44" s="1">
+        <v>1186</v>
+      </c>
+      <c r="AU44" s="1">
+        <v>907</v>
+      </c>
+      <c r="AV44" s="1">
+        <v>1196</v>
+      </c>
+      <c r="AW44" s="1">
+        <v>1624</v>
+      </c>
+      <c r="AX44" s="1">
+        <v>2374</v>
+      </c>
+      <c r="AY44" s="1">
+        <v>8144</v>
+      </c>
+      <c r="AZ44" s="1">
+        <v>8024</v>
+      </c>
+      <c r="BA44" s="1">
+        <v>8055</v>
+      </c>
+      <c r="BB44" s="1">
+        <v>12633</v>
+      </c>
+      <c r="BC44" s="1">
+        <v>11173</v>
+      </c>
+      <c r="BD44" s="1">
+        <v>10755</v>
+      </c>
+      <c r="BE44" s="1">
+        <v>13352</v>
+      </c>
+      <c r="BF44" s="1">
+        <v>12418</v>
+      </c>
+      <c r="BG44" s="1">
+        <v>12266</v>
+      </c>
+      <c r="BH44" s="1">
+        <v>12020</v>
+      </c>
+      <c r="BI44" s="1">
+        <v>13104</v>
+      </c>
+    </row>
+    <row r="45" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V45" s="1">
+        <v>6406</v>
+      </c>
+      <c r="W45" s="1">
+        <v>6305</v>
+      </c>
+      <c r="X45" s="1">
+        <v>4770</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>5007</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>5350</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>4226</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>4494</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>3774</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>3980</v>
+      </c>
+      <c r="AE45" s="1">
+        <v>3942</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>5447</v>
+      </c>
+      <c r="AG45" s="1">
+        <v>4097</v>
+      </c>
+      <c r="AH45" s="1">
+        <v>5636</v>
+      </c>
+      <c r="AI45" s="1">
+        <v>2790</v>
+      </c>
+      <c r="AJ45" s="1">
+        <v>2932</v>
+      </c>
+      <c r="AK45" s="1">
+        <v>3986</v>
+      </c>
+      <c r="AL45" s="1">
+        <v>3378</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>3137</v>
+      </c>
+      <c r="AN45" s="1">
+        <v>1597</v>
+      </c>
+      <c r="AO45" s="1">
+        <v>2243</v>
+      </c>
+      <c r="AP45" s="1">
+        <v>1291</v>
+      </c>
+      <c r="AQ45" s="1">
+        <v>1802</v>
+      </c>
+      <c r="AR45" s="1">
+        <v>3085</v>
+      </c>
+      <c r="AS45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="1">
+        <v>1134</v>
+      </c>
+      <c r="AU45" s="1">
+        <v>855</v>
+      </c>
+      <c r="AV45" s="1">
+        <v>1143</v>
+      </c>
+      <c r="AW45" s="1">
+        <v>1572</v>
+      </c>
+      <c r="AX45" s="1">
+        <v>2321</v>
+      </c>
+      <c r="AY45" s="1">
+        <v>8092</v>
+      </c>
+      <c r="AZ45" s="1">
+        <v>7972</v>
+      </c>
+      <c r="BA45" s="1">
+        <v>8003</v>
+      </c>
+      <c r="BB45" s="1">
+        <v>12580</v>
+      </c>
+      <c r="BC45" s="1">
+        <v>11121</v>
+      </c>
+      <c r="BD45" s="1">
+        <v>10702</v>
+      </c>
+      <c r="BE45" s="1">
+        <v>13299</v>
+      </c>
+      <c r="BF45" s="1">
+        <v>12366</v>
+      </c>
+      <c r="BG45" s="1">
+        <v>12214</v>
+      </c>
+      <c r="BH45" s="1">
+        <v>11967</v>
+      </c>
+      <c r="BI45" s="1">
+        <v>13051</v>
+      </c>
+    </row>
+    <row r="46" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V46" s="1">
+        <v>6362</v>
+      </c>
+      <c r="W46" s="1">
+        <v>6260</v>
+      </c>
+      <c r="X46" s="1">
+        <v>4725</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>4963</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>5305</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>4182</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>4449</v>
+      </c>
+      <c r="AC46" s="1">
+        <v>3730</v>
+      </c>
+      <c r="AD46" s="1">
+        <v>3936</v>
+      </c>
+      <c r="AE46" s="1">
+        <v>3897</v>
+      </c>
+      <c r="AF46" s="1">
+        <v>5402</v>
+      </c>
+      <c r="AG46" s="1">
+        <v>4052</v>
+      </c>
+      <c r="AH46" s="1">
+        <v>5591</v>
+      </c>
+      <c r="AI46" s="1">
+        <v>2745</v>
+      </c>
+      <c r="AJ46" s="1">
+        <v>2887</v>
+      </c>
+      <c r="AK46" s="1">
+        <v>3941</v>
+      </c>
+      <c r="AL46" s="1">
+        <v>3334</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>3092</v>
+      </c>
+      <c r="AN46" s="1">
+        <v>1552</v>
+      </c>
+      <c r="AO46" s="1">
+        <v>2199</v>
+      </c>
+      <c r="AP46" s="1">
+        <v>1247</v>
+      </c>
+      <c r="AQ46" s="1">
+        <v>1757</v>
+      </c>
+      <c r="AR46" s="1">
+        <v>3040</v>
+      </c>
+      <c r="AS46" s="1">
+        <v>3145</v>
+      </c>
+      <c r="AT46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU46" s="1">
+        <v>810</v>
+      </c>
+      <c r="AV46" s="1">
+        <v>1098</v>
+      </c>
+      <c r="AW46" s="1">
+        <v>1527</v>
+      </c>
+      <c r="AX46" s="1">
+        <v>2276</v>
+      </c>
+      <c r="AY46" s="1">
+        <v>8047</v>
+      </c>
+      <c r="AZ46" s="1">
+        <v>7927</v>
+      </c>
+      <c r="BA46" s="1">
+        <v>7958</v>
+      </c>
+      <c r="BB46" s="1">
+        <v>12536</v>
+      </c>
+      <c r="BC46" s="1">
+        <v>11076</v>
+      </c>
+      <c r="BD46" s="1">
+        <v>10658</v>
+      </c>
+      <c r="BE46" s="1">
+        <v>13255</v>
+      </c>
+      <c r="BF46" s="1">
+        <v>12321</v>
+      </c>
+      <c r="BG46" s="1">
+        <v>12169</v>
+      </c>
+      <c r="BH46" s="1">
+        <v>11923</v>
+      </c>
+      <c r="BI46" s="1">
+        <v>13007</v>
+      </c>
+    </row>
+    <row r="47" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V47" s="1">
+        <v>8689</v>
+      </c>
+      <c r="W47" s="1">
+        <v>5767</v>
+      </c>
+      <c r="X47" s="1">
+        <v>4871</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>5108</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>7633</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>4327</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>4595</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>6057</v>
+      </c>
+      <c r="AD47" s="1">
+        <v>6263</v>
+      </c>
+      <c r="AE47" s="1">
+        <v>6224</v>
+      </c>
+      <c r="AF47" s="1">
+        <v>9024</v>
+      </c>
+      <c r="AG47" s="1">
+        <v>6379</v>
+      </c>
+      <c r="AH47" s="1">
+        <v>7918</v>
+      </c>
+      <c r="AI47" s="1">
+        <v>5073</v>
+      </c>
+      <c r="AJ47" s="1">
+        <v>5214</v>
+      </c>
+      <c r="AK47" s="1">
+        <v>6265</v>
+      </c>
+      <c r="AL47" s="1">
+        <v>5661</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>5417</v>
+      </c>
+      <c r="AN47" s="1">
+        <v>3879</v>
+      </c>
+      <c r="AO47" s="1">
+        <v>4526</v>
+      </c>
+      <c r="AP47" s="1">
+        <v>3574</v>
+      </c>
+      <c r="AQ47" s="1">
+        <v>947</v>
+      </c>
+      <c r="AR47" s="1">
+        <v>2230</v>
+      </c>
+      <c r="AS47" s="1">
+        <v>2335</v>
+      </c>
+      <c r="AT47" s="1">
+        <v>112</v>
+      </c>
+      <c r="AU47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="1">
+        <v>288</v>
+      </c>
+      <c r="AW47" s="1">
+        <v>717</v>
+      </c>
+      <c r="AX47" s="1">
+        <v>1461</v>
+      </c>
+      <c r="AY47" s="1">
+        <v>6171</v>
+      </c>
+      <c r="AZ47" s="1">
+        <v>7118</v>
+      </c>
+      <c r="BA47" s="1">
+        <v>7149</v>
+      </c>
+      <c r="BB47" s="1">
+        <v>14225</v>
+      </c>
+      <c r="BC47" s="1">
+        <v>8194</v>
+      </c>
+      <c r="BD47" s="1">
+        <v>7748</v>
+      </c>
+      <c r="BE47" s="1">
+        <v>11742</v>
+      </c>
+      <c r="BF47" s="1">
+        <v>11512</v>
+      </c>
+      <c r="BG47" s="1">
+        <v>11360</v>
+      </c>
+      <c r="BH47" s="1">
+        <v>11114</v>
+      </c>
+      <c r="BI47" s="1">
+        <v>12198</v>
+      </c>
+    </row>
+    <row r="48" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V48" s="1">
+        <v>8401</v>
+      </c>
+      <c r="W48" s="1">
+        <v>5479</v>
+      </c>
+      <c r="X48" s="1">
+        <v>4583</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>4820</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>7344</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>4039</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>4306</v>
+      </c>
+      <c r="AC48" s="1">
+        <v>5769</v>
+      </c>
+      <c r="AD48" s="1">
+        <v>5975</v>
+      </c>
+      <c r="AE48" s="1">
+        <v>5936</v>
+      </c>
+      <c r="AF48" s="1">
+        <v>8735</v>
+      </c>
+      <c r="AG48" s="1">
+        <v>6091</v>
+      </c>
+      <c r="AH48" s="1">
+        <v>7630</v>
+      </c>
+      <c r="AI48" s="1">
+        <v>4784</v>
+      </c>
+      <c r="AJ48" s="1">
+        <v>4926</v>
+      </c>
+      <c r="AK48" s="1">
+        <v>5977</v>
+      </c>
+      <c r="AL48" s="1">
+        <v>5373</v>
+      </c>
+      <c r="AM48" s="1">
+        <v>5129</v>
+      </c>
+      <c r="AN48" s="1">
+        <v>3591</v>
+      </c>
+      <c r="AO48" s="1">
+        <v>4237</v>
+      </c>
+      <c r="AP48" s="1">
+        <v>3286</v>
+      </c>
+      <c r="AQ48" s="1">
+        <v>659</v>
+      </c>
+      <c r="AR48" s="1">
+        <v>1942</v>
+      </c>
+      <c r="AS48" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AT48" s="1">
+        <v>2371</v>
+      </c>
+      <c r="AU48" s="1">
+        <v>2849</v>
+      </c>
+      <c r="AV48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW48" s="1">
+        <v>429</v>
+      </c>
+      <c r="AX48" s="1">
+        <v>1173</v>
+      </c>
+      <c r="AY48" s="1">
+        <v>5883</v>
+      </c>
+      <c r="AZ48" s="1">
+        <v>6830</v>
+      </c>
+      <c r="BA48" s="1">
+        <v>6861</v>
+      </c>
+      <c r="BB48" s="1">
+        <v>13936</v>
+      </c>
+      <c r="BC48" s="1">
+        <v>7906</v>
+      </c>
+      <c r="BD48" s="1">
+        <v>7459</v>
+      </c>
+      <c r="BE48" s="1">
+        <v>11454</v>
+      </c>
+      <c r="BF48" s="1">
+        <v>11224</v>
+      </c>
+      <c r="BG48" s="1">
+        <v>11072</v>
+      </c>
+      <c r="BH48" s="1">
+        <v>10825</v>
+      </c>
+      <c r="BI48" s="1">
+        <v>11909</v>
+      </c>
+    </row>
+    <row r="49" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V49" s="1">
+        <v>7972</v>
+      </c>
+      <c r="W49" s="1">
+        <v>5050</v>
+      </c>
+      <c r="X49" s="1">
+        <v>4154</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>4391</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>6916</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>3610</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>3878</v>
+      </c>
+      <c r="AC49" s="1">
+        <v>5340</v>
+      </c>
+      <c r="AD49" s="1">
+        <v>5546</v>
+      </c>
+      <c r="AE49" s="1">
+        <v>5507</v>
+      </c>
+      <c r="AF49" s="1">
+        <v>8307</v>
+      </c>
+      <c r="AG49" s="1">
+        <v>5662</v>
+      </c>
+      <c r="AH49" s="1">
+        <v>7201</v>
+      </c>
+      <c r="AI49" s="1">
+        <v>4356</v>
+      </c>
+      <c r="AJ49" s="1">
+        <v>4497</v>
+      </c>
+      <c r="AK49" s="1">
+        <v>5548</v>
+      </c>
+      <c r="AL49" s="1">
+        <v>4944</v>
+      </c>
+      <c r="AM49" s="1">
+        <v>4700</v>
+      </c>
+      <c r="AN49" s="1">
+        <v>3162</v>
+      </c>
+      <c r="AO49" s="1">
+        <v>3809</v>
+      </c>
+      <c r="AP49" s="1">
+        <v>2857</v>
+      </c>
+      <c r="AQ49" s="1">
+        <v>438</v>
+      </c>
+      <c r="AR49" s="1">
+        <v>1513</v>
+      </c>
+      <c r="AS49" s="1">
+        <v>1618</v>
+      </c>
+      <c r="AT49" s="1">
+        <v>1942</v>
+      </c>
+      <c r="AU49" s="1">
+        <v>2420</v>
+      </c>
+      <c r="AV49" s="1">
+        <v>2708</v>
+      </c>
+      <c r="AW49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX49" s="1">
+        <v>1152</v>
+      </c>
+      <c r="AY49" s="1">
+        <v>6155</v>
+      </c>
+      <c r="AZ49" s="1">
+        <v>7102</v>
+      </c>
+      <c r="BA49" s="1">
+        <v>7133</v>
+      </c>
+      <c r="BB49" s="1">
+        <v>14146</v>
+      </c>
+      <c r="BC49" s="1">
+        <v>8178</v>
+      </c>
+      <c r="BD49" s="1">
+        <v>7731</v>
+      </c>
+      <c r="BE49" s="1">
+        <v>11726</v>
+      </c>
+      <c r="BF49" s="1">
+        <v>11496</v>
+      </c>
+      <c r="BG49" s="1">
+        <v>11344</v>
+      </c>
+      <c r="BH49" s="1">
+        <v>11097</v>
+      </c>
+      <c r="BI49" s="1">
+        <v>12181</v>
+      </c>
+    </row>
+    <row r="50" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V50" s="1">
+        <v>4786</v>
+      </c>
+      <c r="W50" s="1">
+        <v>4649</v>
+      </c>
+      <c r="X50" s="1">
+        <v>3752</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>3990</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>3730</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>3209</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>3476</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>5292</v>
+      </c>
+      <c r="AD50" s="1">
+        <v>5498</v>
+      </c>
+      <c r="AE50" s="1">
+        <v>5459</v>
+      </c>
+      <c r="AF50" s="1">
+        <v>6965</v>
+      </c>
+      <c r="AG50" s="1">
+        <v>5615</v>
+      </c>
+      <c r="AH50" s="1">
+        <v>7153</v>
+      </c>
+      <c r="AI50" s="1">
+        <v>4308</v>
+      </c>
+      <c r="AJ50" s="1">
+        <v>4449</v>
+      </c>
+      <c r="AK50" s="1">
+        <v>5520</v>
+      </c>
+      <c r="AL50" s="1">
+        <v>4896</v>
+      </c>
+      <c r="AM50" s="1">
+        <v>4672</v>
+      </c>
+      <c r="AN50" s="1">
+        <v>3114</v>
+      </c>
+      <c r="AO50" s="1">
+        <v>3761</v>
+      </c>
+      <c r="AP50" s="1">
+        <v>3172</v>
+      </c>
+      <c r="AQ50" s="1">
+        <v>1587</v>
+      </c>
+      <c r="AR50" s="1">
+        <v>2123</v>
+      </c>
+      <c r="AS50" s="1">
+        <v>2228</v>
+      </c>
+      <c r="AT50" s="1">
+        <v>2552</v>
+      </c>
+      <c r="AU50" s="1">
+        <v>2704</v>
+      </c>
+      <c r="AV50" s="1">
+        <v>2992</v>
+      </c>
+      <c r="AW50" s="1">
+        <v>1148</v>
+      </c>
+      <c r="AX50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY50" s="1">
+        <v>5180</v>
+      </c>
+      <c r="AZ50" s="1">
+        <v>6134</v>
+      </c>
+      <c r="BA50" s="1">
+        <v>6165</v>
+      </c>
+      <c r="BB50" s="1">
+        <v>13240</v>
+      </c>
+      <c r="BC50" s="1">
+        <v>7203</v>
+      </c>
+      <c r="BD50" s="1">
+        <v>6756</v>
+      </c>
+      <c r="BE50" s="1">
+        <v>10758</v>
+      </c>
+      <c r="BF50" s="1">
+        <v>10528</v>
+      </c>
+      <c r="BG50" s="1">
+        <v>10376</v>
+      </c>
+      <c r="BH50" s="1">
+        <v>10129</v>
+      </c>
+      <c r="BI50" s="1">
+        <v>11213</v>
+      </c>
+    </row>
+    <row r="51" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V51" s="1">
+        <v>6571</v>
+      </c>
+      <c r="W51" s="1">
+        <v>6540</v>
+      </c>
+      <c r="X51" s="1">
+        <v>7103</v>
+      </c>
+      <c r="Y51" s="1">
+        <v>7141</v>
+      </c>
+      <c r="Z51" s="1">
+        <v>8041</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>7687</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>7840</v>
+      </c>
+      <c r="AC51" s="1">
+        <v>9597</v>
+      </c>
+      <c r="AD51" s="1">
+        <v>10248</v>
+      </c>
+      <c r="AE51" s="1">
+        <v>10209</v>
+      </c>
+      <c r="AF51" s="1">
+        <v>13886</v>
+      </c>
+      <c r="AG51" s="1">
+        <v>10364</v>
+      </c>
+      <c r="AH51" s="1">
+        <v>11903</v>
+      </c>
+      <c r="AI51" s="1">
+        <v>10075</v>
+      </c>
+      <c r="AJ51" s="1">
+        <v>10217</v>
+      </c>
+      <c r="AK51" s="1">
+        <v>11262</v>
+      </c>
+      <c r="AL51" s="1">
+        <v>10663</v>
+      </c>
+      <c r="AM51" s="1">
+        <v>10413</v>
+      </c>
+      <c r="AN51" s="1">
+        <v>8882</v>
+      </c>
+      <c r="AO51" s="1">
+        <v>9528</v>
+      </c>
+      <c r="AP51" s="1">
+        <v>8576</v>
+      </c>
+      <c r="AQ51" s="1">
+        <v>7195</v>
+      </c>
+      <c r="AR51" s="1">
+        <v>7225</v>
+      </c>
+      <c r="AS51" s="1">
+        <v>7337</v>
+      </c>
+      <c r="AT51" s="1">
+        <v>7653</v>
+      </c>
+      <c r="AU51" s="1">
+        <v>8140</v>
+      </c>
+      <c r="AV51" s="1">
+        <v>8428</v>
+      </c>
+      <c r="AW51" s="1">
+        <v>7295</v>
+      </c>
+      <c r="AX51" s="1">
+        <v>7261</v>
+      </c>
+      <c r="AY51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ51" s="1">
+        <v>2701</v>
+      </c>
+      <c r="BA51" s="1">
+        <v>2732</v>
+      </c>
+      <c r="BB51" s="1">
+        <v>3848</v>
+      </c>
+      <c r="BC51" s="1">
+        <v>3518</v>
+      </c>
+      <c r="BD51" s="1">
+        <v>3071</v>
+      </c>
+      <c r="BE51" s="1">
+        <v>5259</v>
+      </c>
+      <c r="BF51" s="1">
+        <v>4405</v>
+      </c>
+      <c r="BG51" s="1">
+        <v>7144</v>
+      </c>
+      <c r="BH51" s="1">
+        <v>6898</v>
+      </c>
+      <c r="BI51" s="1">
+        <v>7982</v>
+      </c>
+    </row>
+    <row r="52" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V52" s="1">
+        <v>8138</v>
+      </c>
+      <c r="W52" s="1">
+        <v>8107</v>
+      </c>
+      <c r="X52" s="1">
+        <v>8669</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>8708</v>
+      </c>
+      <c r="Z52" s="1">
+        <v>9608</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>9254</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>9406</v>
+      </c>
+      <c r="AC52" s="1">
+        <v>11163</v>
+      </c>
+      <c r="AD52" s="1">
+        <v>11814</v>
+      </c>
+      <c r="AE52" s="1">
+        <v>11776</v>
+      </c>
+      <c r="AF52" s="1">
+        <v>14239</v>
+      </c>
+      <c r="AG52" s="1">
+        <v>11931</v>
+      </c>
+      <c r="AH52" s="1">
+        <v>13470</v>
+      </c>
+      <c r="AI52" s="1">
+        <v>11273</v>
+      </c>
+      <c r="AJ52" s="1">
+        <v>11415</v>
+      </c>
+      <c r="AK52" s="1">
+        <v>11481</v>
+      </c>
+      <c r="AL52" s="1">
+        <v>11861</v>
+      </c>
+      <c r="AM52" s="1">
+        <v>11307</v>
+      </c>
+      <c r="AN52" s="1">
+        <v>10079</v>
+      </c>
+      <c r="AO52" s="1">
+        <v>10726</v>
+      </c>
+      <c r="AP52" s="1">
+        <v>9774</v>
+      </c>
+      <c r="AQ52" s="1">
+        <v>8393</v>
+      </c>
+      <c r="AR52" s="1">
+        <v>8422</v>
+      </c>
+      <c r="AS52" s="1">
+        <v>8535</v>
+      </c>
+      <c r="AT52" s="1">
+        <v>8851</v>
+      </c>
+      <c r="AU52" s="1">
+        <v>9338</v>
+      </c>
+      <c r="AV52" s="1">
+        <v>9626</v>
+      </c>
+      <c r="AW52" s="1">
+        <v>8493</v>
+      </c>
+      <c r="AX52" s="1">
+        <v>8459</v>
+      </c>
+      <c r="AY52" s="1">
+        <v>2912</v>
+      </c>
+      <c r="AZ52" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA52" s="1">
+        <v>716</v>
+      </c>
+      <c r="BB52" s="1">
+        <v>3887</v>
+      </c>
+      <c r="BC52" s="1">
+        <v>3557</v>
+      </c>
+      <c r="BD52" s="1">
+        <v>3110</v>
+      </c>
+      <c r="BE52" s="1">
+        <v>5449</v>
+      </c>
+      <c r="BF52" s="1">
+        <v>4444</v>
+      </c>
+      <c r="BG52" s="1">
+        <v>5129</v>
+      </c>
+      <c r="BH52" s="1">
+        <v>4882</v>
+      </c>
+      <c r="BI52" s="1">
+        <v>5966</v>
+      </c>
+    </row>
+    <row r="53" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V53" s="1">
+        <v>8200</v>
+      </c>
+      <c r="W53" s="1">
+        <v>8170</v>
+      </c>
+      <c r="X53" s="1">
+        <v>8732</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>8770</v>
+      </c>
+      <c r="Z53" s="1">
+        <v>9670</v>
+      </c>
+      <c r="AA53" s="1">
+        <v>9317</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>9469</v>
+      </c>
+      <c r="AC53" s="1">
+        <v>11226</v>
+      </c>
+      <c r="AD53" s="1">
+        <v>11877</v>
+      </c>
+      <c r="AE53" s="1">
+        <v>11838</v>
+      </c>
+      <c r="AF53" s="1">
+        <v>15744</v>
+      </c>
+      <c r="AG53" s="1">
+        <v>11993</v>
+      </c>
+      <c r="AH53" s="1">
+        <v>13532</v>
+      </c>
+      <c r="AI53" s="1">
+        <v>11704</v>
+      </c>
+      <c r="AJ53" s="1">
+        <v>11846</v>
+      </c>
+      <c r="AK53" s="1">
+        <v>12986</v>
+      </c>
+      <c r="AL53" s="1">
+        <v>12293</v>
+      </c>
+      <c r="AM53" s="1">
+        <v>12811</v>
+      </c>
+      <c r="AN53" s="1">
+        <v>10511</v>
+      </c>
+      <c r="AO53" s="1">
+        <v>11157</v>
+      </c>
+      <c r="AP53" s="1">
+        <v>10206</v>
+      </c>
+      <c r="AQ53" s="1">
+        <v>8824</v>
+      </c>
+      <c r="AR53" s="1">
+        <v>8854</v>
+      </c>
+      <c r="AS53" s="1">
+        <v>8967</v>
+      </c>
+      <c r="AT53" s="1">
+        <v>9283</v>
+      </c>
+      <c r="AU53" s="1">
+        <v>9769</v>
+      </c>
+      <c r="AV53" s="1">
+        <v>10057</v>
+      </c>
+      <c r="AW53" s="1">
+        <v>8925</v>
+      </c>
+      <c r="AX53" s="1">
+        <v>8890</v>
+      </c>
+      <c r="AY53" s="1">
+        <v>2700</v>
+      </c>
+      <c r="AZ53" s="1">
+        <v>402</v>
+      </c>
+      <c r="BA53" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB53" s="1">
+        <v>3983</v>
+      </c>
+      <c r="BC53" s="1">
+        <v>3653</v>
+      </c>
+      <c r="BD53" s="1">
+        <v>3206</v>
+      </c>
+      <c r="BE53" s="1">
+        <v>5500</v>
+      </c>
+      <c r="BF53" s="1">
+        <v>4540</v>
+      </c>
+      <c r="BG53" s="1">
+        <v>4488</v>
+      </c>
+      <c r="BH53" s="1">
+        <v>4242</v>
+      </c>
+      <c r="BI53" s="1">
+        <v>5326</v>
+      </c>
+    </row>
+    <row r="54" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V54" s="1">
+        <v>8899</v>
+      </c>
+      <c r="W54" s="1">
+        <v>8868</v>
+      </c>
+      <c r="X54" s="1">
+        <v>9430</v>
+      </c>
+      <c r="Y54" s="1">
+        <v>9469</v>
+      </c>
+      <c r="Z54" s="1">
+        <v>13765</v>
+      </c>
+      <c r="AA54" s="1">
+        <v>13244</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>13511</v>
+      </c>
+      <c r="AC54" s="1">
+        <v>11924</v>
+      </c>
+      <c r="AD54" s="1">
+        <v>12575</v>
+      </c>
+      <c r="AE54" s="1">
+        <v>12537</v>
+      </c>
+      <c r="AF54" s="1">
+        <v>20599</v>
+      </c>
+      <c r="AG54" s="1">
+        <v>12692</v>
+      </c>
+      <c r="AH54" s="1">
+        <v>14231</v>
+      </c>
+      <c r="AI54" s="1">
+        <v>16655</v>
+      </c>
+      <c r="AJ54" s="1">
+        <v>16796</v>
+      </c>
+      <c r="AK54" s="1">
+        <v>17841</v>
+      </c>
+      <c r="AL54" s="1">
+        <v>17243</v>
+      </c>
+      <c r="AM54" s="1">
+        <v>16993</v>
+      </c>
+      <c r="AN54" s="1">
+        <v>15461</v>
+      </c>
+      <c r="AO54" s="1">
+        <v>16108</v>
+      </c>
+      <c r="AP54" s="1">
+        <v>15156</v>
+      </c>
+      <c r="AQ54" s="1">
+        <v>13774</v>
+      </c>
+      <c r="AR54" s="1">
+        <v>13804</v>
+      </c>
+      <c r="AS54" s="1">
+        <v>13917</v>
+      </c>
+      <c r="AT54" s="1">
+        <v>14233</v>
+      </c>
+      <c r="AU54" s="1">
+        <v>14719</v>
+      </c>
+      <c r="AV54" s="1">
+        <v>15008</v>
+      </c>
+      <c r="AW54" s="1">
+        <v>13875</v>
+      </c>
+      <c r="AX54" s="1">
+        <v>13841</v>
+      </c>
+      <c r="AY54" s="1">
+        <v>3393</v>
+      </c>
+      <c r="AZ54" s="1">
+        <v>3685</v>
+      </c>
+      <c r="BA54" s="1">
+        <v>3640</v>
+      </c>
+      <c r="BB54" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC54" s="1">
+        <v>968</v>
+      </c>
+      <c r="BD54" s="1">
+        <v>618</v>
+      </c>
+      <c r="BE54" s="1">
+        <v>2021</v>
+      </c>
+      <c r="BF54" s="1">
+        <v>2294</v>
+      </c>
+      <c r="BG54" s="1">
+        <v>6132</v>
+      </c>
+      <c r="BH54" s="1">
+        <v>5747</v>
+      </c>
+      <c r="BI54" s="1">
+        <v>6027</v>
+      </c>
+    </row>
+    <row r="55" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V55" s="1">
+        <v>7551</v>
+      </c>
+      <c r="W55" s="1">
+        <v>7520</v>
+      </c>
+      <c r="X55" s="1">
+        <v>8082</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>8121</v>
+      </c>
+      <c r="Z55" s="1">
+        <v>9475</v>
+      </c>
+      <c r="AA55" s="1">
+        <v>8953</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>9221</v>
+      </c>
+      <c r="AC55" s="1">
+        <v>10576</v>
+      </c>
+      <c r="AD55" s="1">
+        <v>11227</v>
+      </c>
+      <c r="AE55" s="1">
+        <v>11189</v>
+      </c>
+      <c r="AF55" s="1">
+        <v>16309</v>
+      </c>
+      <c r="AG55" s="1">
+        <v>11344</v>
+      </c>
+      <c r="AH55" s="1">
+        <v>12883</v>
+      </c>
+      <c r="AI55" s="1">
+        <v>12364</v>
+      </c>
+      <c r="AJ55" s="1">
+        <v>12506</v>
+      </c>
+      <c r="AK55" s="1">
+        <v>13551</v>
+      </c>
+      <c r="AL55" s="1">
+        <v>12953</v>
+      </c>
+      <c r="AM55" s="1">
+        <v>12702</v>
+      </c>
+      <c r="AN55" s="1">
+        <v>11171</v>
+      </c>
+      <c r="AO55" s="1">
+        <v>11817</v>
+      </c>
+      <c r="AP55" s="1">
+        <v>10866</v>
+      </c>
+      <c r="AQ55" s="1">
+        <v>9484</v>
+      </c>
+      <c r="AR55" s="1">
+        <v>9514</v>
+      </c>
+      <c r="AS55" s="1">
+        <v>9627</v>
+      </c>
+      <c r="AT55" s="1">
+        <v>9943</v>
+      </c>
+      <c r="AU55" s="1">
+        <v>10429</v>
+      </c>
+      <c r="AV55" s="1">
+        <v>10717</v>
+      </c>
+      <c r="AW55" s="1">
+        <v>9585</v>
+      </c>
+      <c r="AX55" s="1">
+        <v>9550</v>
+      </c>
+      <c r="AY55" s="1">
+        <v>3192</v>
+      </c>
+      <c r="AZ55" s="1">
+        <v>3484</v>
+      </c>
+      <c r="BA55" s="1">
+        <v>3438</v>
+      </c>
+      <c r="BB55" s="1">
+        <v>361</v>
+      </c>
+      <c r="BC55" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD55" s="1">
+        <v>416</v>
+      </c>
+      <c r="BE55" s="1">
+        <v>1883</v>
+      </c>
+      <c r="BF55" s="1">
+        <v>2092</v>
+      </c>
+      <c r="BG55" s="1">
+        <v>5930</v>
+      </c>
+      <c r="BH55" s="1">
+        <v>5545</v>
+      </c>
+      <c r="BI55" s="1">
+        <v>5825</v>
+      </c>
+    </row>
+    <row r="56" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V56" s="1">
+        <v>8281</v>
+      </c>
+      <c r="W56" s="1">
+        <v>8250</v>
+      </c>
+      <c r="X56" s="1">
+        <v>8813</v>
+      </c>
+      <c r="Y56" s="1">
+        <v>8851</v>
+      </c>
+      <c r="Z56" s="1">
+        <v>9751</v>
+      </c>
+      <c r="AA56" s="1">
+        <v>9080</v>
+      </c>
+      <c r="AB56" s="1">
+        <v>9550</v>
+      </c>
+      <c r="AC56" s="1">
+        <v>11307</v>
+      </c>
+      <c r="AD56" s="1">
+        <v>11958</v>
+      </c>
+      <c r="AE56" s="1">
+        <v>11919</v>
+      </c>
+      <c r="AF56" s="1">
+        <v>17319</v>
+      </c>
+      <c r="AG56" s="1">
+        <v>12074</v>
+      </c>
+      <c r="AH56" s="1">
+        <v>13613</v>
+      </c>
+      <c r="AI56" s="1">
+        <v>12491</v>
+      </c>
+      <c r="AJ56" s="1">
+        <v>12633</v>
+      </c>
+      <c r="AK56" s="1">
+        <v>14561</v>
+      </c>
+      <c r="AL56" s="1">
+        <v>13079</v>
+      </c>
+      <c r="AM56" s="1">
+        <v>12829</v>
+      </c>
+      <c r="AN56" s="1">
+        <v>11297</v>
+      </c>
+      <c r="AO56" s="1">
+        <v>11944</v>
+      </c>
+      <c r="AP56" s="1">
+        <v>10992</v>
+      </c>
+      <c r="AQ56" s="1">
+        <v>9611</v>
+      </c>
+      <c r="AR56" s="1">
+        <v>9640</v>
+      </c>
+      <c r="AS56" s="1">
+        <v>9753</v>
+      </c>
+      <c r="AT56" s="1">
+        <v>10069</v>
+      </c>
+      <c r="AU56" s="1">
+        <v>10556</v>
+      </c>
+      <c r="AV56" s="1">
+        <v>10844</v>
+      </c>
+      <c r="AW56" s="1">
+        <v>9711</v>
+      </c>
+      <c r="AX56" s="1">
+        <v>9677</v>
+      </c>
+      <c r="AY56" s="1">
+        <v>2776</v>
+      </c>
+      <c r="AZ56" s="1">
+        <v>3068</v>
+      </c>
+      <c r="BA56" s="1">
+        <v>3022</v>
+      </c>
+      <c r="BB56" s="1">
+        <v>777</v>
+      </c>
+      <c r="BC56" s="1">
+        <v>413</v>
+      </c>
+      <c r="BD56" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE56" s="1">
+        <v>2299</v>
+      </c>
+      <c r="BF56" s="1">
+        <v>1722</v>
+      </c>
+      <c r="BG56" s="1">
+        <v>5515</v>
+      </c>
+      <c r="BH56" s="1">
+        <v>5129</v>
+      </c>
+      <c r="BI56" s="1">
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="57" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V57" s="1">
+        <v>11956</v>
+      </c>
+      <c r="W57" s="1">
+        <v>11926</v>
+      </c>
+      <c r="X57" s="1">
+        <v>12488</v>
+      </c>
+      <c r="Y57" s="1">
+        <v>12526</v>
+      </c>
+      <c r="Z57" s="1">
+        <v>11925</v>
+      </c>
+      <c r="AA57" s="1">
+        <v>11403</v>
+      </c>
+      <c r="AB57" s="1">
+        <v>11671</v>
+      </c>
+      <c r="AC57" s="1">
+        <v>14982</v>
+      </c>
+      <c r="AD57" s="1">
+        <v>16005</v>
+      </c>
+      <c r="AE57" s="1">
+        <v>15966</v>
+      </c>
+      <c r="AF57" s="1">
+        <v>18759</v>
+      </c>
+      <c r="AG57" s="1">
+        <v>16121</v>
+      </c>
+      <c r="AH57" s="1">
+        <v>17660</v>
+      </c>
+      <c r="AI57" s="1">
+        <v>14814</v>
+      </c>
+      <c r="AJ57" s="1">
+        <v>14956</v>
+      </c>
+      <c r="AK57" s="1">
+        <v>16001</v>
+      </c>
+      <c r="AL57" s="1">
+        <v>15403</v>
+      </c>
+      <c r="AM57" s="1">
+        <v>15152</v>
+      </c>
+      <c r="AN57" s="1">
+        <v>13621</v>
+      </c>
+      <c r="AO57" s="1">
+        <v>14267</v>
+      </c>
+      <c r="AP57" s="1">
+        <v>13316</v>
+      </c>
+      <c r="AQ57" s="1">
+        <v>11934</v>
+      </c>
+      <c r="AR57" s="1">
+        <v>11964</v>
+      </c>
+      <c r="AS57" s="1">
+        <v>12077</v>
+      </c>
+      <c r="AT57" s="1">
+        <v>12393</v>
+      </c>
+      <c r="AU57" s="1">
+        <v>12879</v>
+      </c>
+      <c r="AV57" s="1">
+        <v>13167</v>
+      </c>
+      <c r="AW57" s="1">
+        <v>12035</v>
+      </c>
+      <c r="AX57" s="1">
+        <v>12000</v>
+      </c>
+      <c r="AY57" s="1">
+        <v>4627</v>
+      </c>
+      <c r="AZ57" s="1">
+        <v>5197</v>
+      </c>
+      <c r="BA57" s="1">
+        <v>5227</v>
+      </c>
+      <c r="BB57" s="1">
+        <v>2218</v>
+      </c>
+      <c r="BC57" s="1">
+        <v>2639</v>
+      </c>
+      <c r="BD57" s="1">
+        <v>2682</v>
+      </c>
+      <c r="BE57" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF57" s="1">
+        <v>1870</v>
+      </c>
+      <c r="BG57" s="1">
+        <v>8844</v>
+      </c>
+      <c r="BH57" s="1">
+        <v>8085</v>
+      </c>
+      <c r="BI57" s="1">
+        <v>7966</v>
+      </c>
+    </row>
+    <row r="58" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V58" s="1">
+        <v>12806</v>
+      </c>
+      <c r="W58" s="1">
+        <v>12775</v>
+      </c>
+      <c r="X58" s="1">
+        <v>13338</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>13376</v>
+      </c>
+      <c r="Z58" s="1">
+        <v>12774</v>
+      </c>
+      <c r="AA58" s="1">
+        <v>12253</v>
+      </c>
+      <c r="AB58" s="1">
+        <v>12520</v>
+      </c>
+      <c r="AC58" s="1">
+        <v>15832</v>
+      </c>
+      <c r="AD58" s="1">
+        <v>16855</v>
+      </c>
+      <c r="AE58" s="1">
+        <v>16816</v>
+      </c>
+      <c r="AF58" s="1">
+        <v>19609</v>
+      </c>
+      <c r="AG58" s="1">
+        <v>16971</v>
+      </c>
+      <c r="AH58" s="1">
+        <v>18510</v>
+      </c>
+      <c r="AI58" s="1">
+        <v>15664</v>
+      </c>
+      <c r="AJ58" s="1">
+        <v>15806</v>
+      </c>
+      <c r="AK58" s="1">
+        <v>16851</v>
+      </c>
+      <c r="AL58" s="1">
+        <v>16252</v>
+      </c>
+      <c r="AM58" s="1">
+        <v>16002</v>
+      </c>
+      <c r="AN58" s="1">
+        <v>14471</v>
+      </c>
+      <c r="AO58" s="1">
+        <v>15117</v>
+      </c>
+      <c r="AP58" s="1">
+        <v>14166</v>
+      </c>
+      <c r="AQ58" s="1">
+        <v>12784</v>
+      </c>
+      <c r="AR58" s="1">
+        <v>12814</v>
+      </c>
+      <c r="AS58" s="1">
+        <v>12926</v>
+      </c>
+      <c r="AT58" s="1">
+        <v>13242</v>
+      </c>
+      <c r="AU58" s="1">
+        <v>13729</v>
+      </c>
+      <c r="AV58" s="1">
+        <v>14017</v>
+      </c>
+      <c r="AW58" s="1">
+        <v>12885</v>
+      </c>
+      <c r="AX58" s="1">
+        <v>12850</v>
+      </c>
+      <c r="AY58" s="1">
+        <v>4204</v>
+      </c>
+      <c r="AZ58" s="1">
+        <v>4508</v>
+      </c>
+      <c r="BA58" s="1">
+        <v>4462</v>
+      </c>
+      <c r="BB58" s="1">
+        <v>2465</v>
+      </c>
+      <c r="BC58" s="1">
+        <v>2705</v>
+      </c>
+      <c r="BD58" s="1">
+        <v>2638</v>
+      </c>
+      <c r="BE58" s="1">
+        <v>1028</v>
+      </c>
+      <c r="BF58" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG58" s="1">
+        <v>6179</v>
+      </c>
+      <c r="BH58" s="1">
+        <v>5419</v>
+      </c>
+      <c r="BI58" s="1">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="59" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V59" s="1">
+        <v>13634</v>
+      </c>
+      <c r="W59" s="1">
+        <v>13603</v>
+      </c>
+      <c r="X59" s="1">
+        <v>14166</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>14204</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>15104</v>
+      </c>
+      <c r="AA59" s="1">
+        <v>14750</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>14903</v>
+      </c>
+      <c r="AC59" s="1">
+        <v>16660</v>
+      </c>
+      <c r="AD59" s="1">
+        <v>17311</v>
+      </c>
+      <c r="AE59" s="1">
+        <v>17272</v>
+      </c>
+      <c r="AF59" s="1">
+        <v>17766</v>
+      </c>
+      <c r="AG59" s="1">
+        <v>17427</v>
+      </c>
+      <c r="AH59" s="1">
+        <v>18966</v>
+      </c>
+      <c r="AI59" s="1">
+        <v>14276</v>
+      </c>
+      <c r="AJ59" s="1">
+        <v>14417</v>
+      </c>
+      <c r="AK59" s="1">
+        <v>15008</v>
+      </c>
+      <c r="AL59" s="1">
+        <v>14864</v>
+      </c>
+      <c r="AM59" s="1">
+        <v>14834</v>
+      </c>
+      <c r="AN59" s="1">
+        <v>16681</v>
+      </c>
+      <c r="AO59" s="1">
+        <v>13729</v>
+      </c>
+      <c r="AP59" s="1">
+        <v>16904</v>
+      </c>
+      <c r="AQ59" s="1">
+        <v>15523</v>
+      </c>
+      <c r="AR59" s="1">
+        <v>15552</v>
+      </c>
+      <c r="AS59" s="1">
+        <v>15665</v>
+      </c>
+      <c r="AT59" s="1">
+        <v>15981</v>
+      </c>
+      <c r="AU59" s="1">
+        <v>16468</v>
+      </c>
+      <c r="AV59" s="1">
+        <v>16756</v>
+      </c>
+      <c r="AW59" s="1">
+        <v>15623</v>
+      </c>
+      <c r="AX59" s="1">
+        <v>15589</v>
+      </c>
+      <c r="AY59" s="1">
+        <v>6992</v>
+      </c>
+      <c r="AZ59" s="1">
+        <v>4969</v>
+      </c>
+      <c r="BA59" s="1">
+        <v>4923</v>
+      </c>
+      <c r="BB59" s="1">
+        <v>6930</v>
+      </c>
+      <c r="BC59" s="1">
+        <v>6600</v>
+      </c>
+      <c r="BD59" s="1">
+        <v>6153</v>
+      </c>
+      <c r="BE59" s="1">
+        <v>6748</v>
+      </c>
+      <c r="BF59" s="1">
+        <v>5894</v>
+      </c>
+      <c r="BG59" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH59" s="1">
+        <v>605</v>
+      </c>
+      <c r="BI59" s="1">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="60" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V60" s="1">
+        <v>12050</v>
+      </c>
+      <c r="W60" s="1">
+        <v>12019</v>
+      </c>
+      <c r="X60" s="1">
+        <v>12581</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>12620</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>13519</v>
+      </c>
+      <c r="AA60" s="1">
+        <v>13166</v>
+      </c>
+      <c r="AB60" s="1">
+        <v>13318</v>
+      </c>
+      <c r="AC60" s="1">
+        <v>15075</v>
+      </c>
+      <c r="AD60" s="1">
+        <v>15726</v>
+      </c>
+      <c r="AE60" s="1">
+        <v>15687</v>
+      </c>
+      <c r="AF60" s="1">
+        <v>18264</v>
+      </c>
+      <c r="AG60" s="1">
+        <v>15843</v>
+      </c>
+      <c r="AH60" s="1">
+        <v>17381</v>
+      </c>
+      <c r="AI60" s="1">
+        <v>13852</v>
+      </c>
+      <c r="AJ60" s="1">
+        <v>13993</v>
+      </c>
+      <c r="AK60" s="1">
+        <v>15506</v>
+      </c>
+      <c r="AL60" s="1">
+        <v>14440</v>
+      </c>
+      <c r="AM60" s="1">
+        <v>15332</v>
+      </c>
+      <c r="AN60" s="1">
+        <v>12658</v>
+      </c>
+      <c r="AO60" s="1">
+        <v>13305</v>
+      </c>
+      <c r="AP60" s="1">
+        <v>16481</v>
+      </c>
+      <c r="AQ60" s="1">
+        <v>15099</v>
+      </c>
+      <c r="AR60" s="1">
+        <v>15129</v>
+      </c>
+      <c r="AS60" s="1">
+        <v>15241</v>
+      </c>
+      <c r="AT60" s="1">
+        <v>15557</v>
+      </c>
+      <c r="AU60" s="1">
+        <v>16044</v>
+      </c>
+      <c r="AV60" s="1">
+        <v>16332</v>
+      </c>
+      <c r="AW60" s="1">
+        <v>15200</v>
+      </c>
+      <c r="AX60" s="1">
+        <v>15165</v>
+      </c>
+      <c r="AY60" s="1">
+        <v>6550</v>
+      </c>
+      <c r="AZ60" s="1">
+        <v>4527</v>
+      </c>
+      <c r="BA60" s="1">
+        <v>4481</v>
+      </c>
+      <c r="BB60" s="1">
+        <v>6470</v>
+      </c>
+      <c r="BC60" s="1">
+        <v>5250</v>
+      </c>
+      <c r="BD60" s="1">
+        <v>5693</v>
+      </c>
+      <c r="BE60" s="1">
+        <v>6283</v>
+      </c>
+      <c r="BF60" s="1">
+        <v>5429</v>
+      </c>
+      <c r="BG60" s="1">
+        <v>386</v>
+      </c>
+      <c r="BH60" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI60" s="1">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="61" spans="22:61" x14ac:dyDescent="0.25">
+      <c r="V61" s="1">
+        <v>14515</v>
+      </c>
+      <c r="W61" s="1">
+        <v>14485</v>
+      </c>
+      <c r="X61" s="1">
+        <v>15047</v>
+      </c>
+      <c r="Y61" s="1">
+        <v>15085</v>
+      </c>
+      <c r="Z61" s="1">
+        <v>15985</v>
+      </c>
+      <c r="AA61" s="1">
+        <v>15632</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>15784</v>
+      </c>
+      <c r="AC61" s="1">
+        <v>17541</v>
+      </c>
+      <c r="AD61" s="1">
+        <v>18192</v>
+      </c>
+      <c r="AE61" s="1">
+        <v>18153</v>
+      </c>
+      <c r="AF61" s="1">
+        <v>18647</v>
+      </c>
+      <c r="AG61" s="1">
+        <v>18308</v>
+      </c>
+      <c r="AH61" s="1">
+        <v>19847</v>
+      </c>
+      <c r="AI61" s="1">
+        <v>15157</v>
+      </c>
+      <c r="AJ61" s="1">
+        <v>15298</v>
+      </c>
+      <c r="AK61" s="1">
+        <v>15889</v>
+      </c>
+      <c r="AL61" s="1">
+        <v>15745</v>
+      </c>
+      <c r="AM61" s="1">
+        <v>15715</v>
+      </c>
+      <c r="AN61" s="1">
+        <v>17562</v>
+      </c>
+      <c r="AO61" s="1">
+        <v>14610</v>
+      </c>
+      <c r="AP61" s="1">
+        <v>17786</v>
+      </c>
+      <c r="AQ61" s="1">
+        <v>16404</v>
+      </c>
+      <c r="AR61" s="1">
+        <v>16434</v>
+      </c>
+      <c r="AS61" s="1">
+        <v>16546</v>
+      </c>
+      <c r="AT61" s="1">
+        <v>16863</v>
+      </c>
+      <c r="AU61" s="1">
+        <v>17349</v>
+      </c>
+      <c r="AV61" s="1">
+        <v>17637</v>
+      </c>
+      <c r="AW61" s="1">
+        <v>16505</v>
+      </c>
+      <c r="AX61" s="1">
+        <v>16470</v>
+      </c>
+      <c r="AY61" s="1">
+        <v>7873</v>
+      </c>
+      <c r="AZ61" s="1">
+        <v>5850</v>
+      </c>
+      <c r="BA61" s="1">
+        <v>5805</v>
+      </c>
+      <c r="BB61" s="1">
+        <v>7811</v>
+      </c>
+      <c r="BC61" s="1">
+        <v>6306</v>
+      </c>
+      <c r="BD61" s="1">
+        <v>7034</v>
+      </c>
+      <c r="BE61" s="1">
+        <v>5635</v>
+      </c>
+      <c r="BF61" s="1">
+        <v>6484</v>
+      </c>
+      <c r="BG61" s="1">
+        <v>1379</v>
+      </c>
+      <c r="BH61" s="1">
+        <v>1195</v>
+      </c>
+      <c r="BI61" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>